<commit_message>
Clean up project files and remove deprecated notebooks and images
- Delete old notebooks: llm_review.ipynb
- Remove unused image files: image-1.png, image-2.png, image-3.png, image.png
- Remove temporary Excel files from data directory
- Comment out data export code in llm_review_v2.ipynb
- Minor cleanup of project structure and unnecessary files
</commit_message>
<xml_diff>
--- a/data/pycon_2024_proposal_with_llm_and_review_0217.xlsx
+++ b/data/pycon_2024_proposal_with_llm_and_review_0217.xlsx
@@ -665,12 +665,13 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>The proposal introduces Python's role in genomics, focusing on variant analysis with scikit-allel and QMplot. More specific examples and details on machine learning applications would improve the proposal.</t>
+          <t>The proposal discusses using Python packages like scikit-allel and QMplot for analyzing and visualizing genetic variants from VCF files. It aims to introduce Python's role in genomics research, particularly in identifying and interpreting mutations, and is targeted towards those interested in applying coding and machine learning skills to bioscience.</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>This proposal introduces the use of Python in genomics, specifically for variant analysis using packages like scikit-allel and QMplot. It highlights the application of Python in analyzing large-scale genetic variation data and visualizing mutations. The talk aims to inform the Python community about the application of Python in genomics research and inspire developers to work in the intersection of computer science and genomics. The outline is clear and the objective is well-defined. However, the proposal could benefit from more specific examples of how these packages are used and the challenges they address. Adding more details on the machine learning aspects mentioned in the objective would also strengthen the proposal.</t>
+          <t xml:space="preserve">This proposal introduces the use of Python in genomics, specifically for variant analysis using packages like scikit-allel and QMplot. It explains how these tools can be used to analyze and visualize genetic variation data. The talk aims to inform the Python community about the application of Python in genomics research and inspire developers to work at the intersection of computer science and genomics. While the topic is interesting, the proposal could benefit from more concrete examples and a deeper dive into the technical challenges and solutions within the Python code. Highlighting specific code snippets and demonstrating how these packages address real-world problems would enhance the talk's practical value. Also, elaborating on the machine learning aspects mentioned in the objective would strengthen the proposal.
+</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -805,12 +806,12 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>The proposal outlines challenges and solutions for testing autonomous mobile robots with Python. More specific Python implementation details would improve the proposal.</t>
+          <t>The proposal discusses the challenges and solutions for testing autonomous mobile robots in warehouse automation, focusing on test automation, simulation, and code quality. It aims to provide insights into ensuring the performance and quality of robotics systems using Python.</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>This proposal discusses testing autonomous mobile robots using Python in warehouse automation. It identifies key challenges like hardware dependency, testability, and non-functional aspects. The solutions proposed, such as test simulation and evidence collection, are relevant. However, the proposal could benefit from more specific examples of Python code used in test automation and details on the frameworks or libraries employed. Expanding on the implementation details would enhance the technical depth and practical value for the audience.</t>
+          <t>This proposal discusses testing autonomous mobile robots, which is relevant to Python due to its use in robotics and automation. The proposal outlines challenges in testing such systems and suggests solutions like test simulation and improving code quality. However, the proposal could benefit from more specific examples of how Python is used in the test automation framework and the tools/libraries employed. Detailing the implementation with Python would strengthen the connection to the PyCon audience. Also, elaborating on the 'Evidence Collection and ROS Bag' point would be beneficial. The outline is a bit high-level and could be more detailed.</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
@@ -933,13 +934,18 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>提案主題實用，結合 Python 和 ML 分析軟體缺陷。但技術深度可能不足，建議加入更多實作細節和案例。</t>
+          <t>The proposal discusses using bug analysis and ML to improve software quality. It aims to present ways to analyze defects and use ML for defect management, but lacks specific details on Python implementation.</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t xml:space="preserve">這個提案探討了如何利用 Python 和機器學習分析軟體缺陷，從而提升軟體品質和測試效率。優點是主題具有實用性，並結合了 Python 和 ML 技術。缺點是技術深度可能不足，需要更具體的實作細節，例如使用的 ML 演算法、資料處理流程等。建議在演講中加入實際案例和實驗數據，以增強說服力。此外，可以更詳細地介紹如何將分析結果應用於持續改進。
-</t>
+          <t>The proposal discusses bug analysis and using ML to improve software quality. While the topic is interesting, the proposal needs to clearly demonstrate the use of Python. The outline mentions a "Python System which reads bugs from Issue tracking system and classifies", but the abstract and detailed description lack specific details about the Python code, libraries (e.g., data analysis, ML frameworks), and implementation. To improve, the proposal should include concrete examples of how Python is used to extract, analyze, and visualize bug data. Without a stronger Python focus, it might be better suited for a general software engineering conference.
+Consider adding details about:
+- Specific Python libraries used (e.g., pandas, scikit-learn, matplotlib).
+- Code snippets demonstrating data extraction and analysis.
+- Examples of ML models used for bug classification.
+- Visualizations generated using Python.
+Without these details, the proposal is currently weak.</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
@@ -1063,12 +1069,12 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Good application of RAG for documentation, but needs more Python and technical depth.</t>
+          <t>This proposal discusses using Retrieval Augmented Generation (RAG) with Amazon Bedrock to create dynamic knowledge bases for technical documentation. It involves using Python to interact with Amazon Bedrock's APIs. The proposal includes a live demonstration of a documentation generation system.</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>This proposal introduces an interesting application of RAG with Amazon Bedrock for technical documentation. It highlights a practical use case of generative AI in a domain relevant to many developers. The outline is well-structured, and the live demonstration promises to be engaging. However, the proposal could benefit from a deeper dive into the specific Python libraries and techniques used to interact with Amazon Bedrock's APIs. Detailing the challenges faced and solutions implemented during the RAG integration would also enhance the technical depth. Consider adding more specifics on how the data sources are processed and prepared for RAG. Also, while the use of AWS services is mentioned, elaborating on the specific services and their roles would be beneficial.</t>
+          <t>This proposal introduces an innovative approach to technical documentation using Retrieval Augmented Generation (RAG) with Amazon Bedrock. It outlines the use of Python to interact with Amazon Bedrock's APIs for data retrieval and content generation. The live demonstration of a documentation generation system is a strong point. However, the proposal could benefit from more specific details on the Python code involved and the challenges faced during implementation. Also, while Amazon Bedrock is mentioned, the proposal could better highlight the Python-specific aspects of interacting with this service. Consider adding more details on specific Python libraries or frameworks used. The proposal is generally well-structured, but the connection to the broader Python ecosystem could be strengthened.</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1209,12 +1215,12 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Interesting mathematical approach to LeetCode problems, but the connection to Python needs to be strengthened with more concrete examples and performance comparisons.</t>
+          <t>The proposal explores solving LeetCode problems using mathematical methods like Tree Diagrams, Unique Path Count, and Pascal's Triangle with Binomial Expansion, focusing on LeetCode Problem 808. It aims to optimize runtime and memory usage, providing Python code snippets for implementation.</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>This proposal presents an interesting approach to solving LeetCode problems using mathematical methods. While the application of Pascal's Triangle and Binomial Expansion is intriguing, the connection to Python is somewhat weak. The proposal could be strengthened by demonstrating how Python can be used to efficiently implement these mathematical solutions and compare their performance against traditional algorithmic approaches. The current Python code snippets are mentioned but not detailed enough. To improve, the talk should include more concrete Python examples and benchmarks. Consider focusing on the practical implementation and optimization of the mathematical solution in Python.</t>
+          <t>This proposal presents an interesting approach to solving LeetCode problems using mathematical techniques. While the application of Pascal's Triangle and Binomial Expansion is intriguing, the connection to Python could be strengthened. The proposal could benefit from more explicit Python code examples demonstrating the implementation of the closed-form solution and comparing its performance against other Python-based approaches. To better align with the PyCon audience, consider emphasizing the practical application of these mathematical concepts within a Python coding context, showcasing how they can optimize Python code for specific problem types. Also, the target audience seems a bit narrow. Consider broadening the appeal to Python developers interested in algorithm optimization.</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
@@ -1348,14 +1354,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>提案將 MicroPython 應用於訓練狗狗，有趣且具潛力。建議深入探討技術細節，並明確說明專案對 Python 社群的價值。</t>
+          <t>This talk explores using MicroPython on ESP32 to train a dog, covering challenges in hardware integration, rapid prototyping, and lessons learned from a hobby project. It touches on logging, power management, and coding principles.</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>這個提案很有趣，將 MicroPython 應用於訓練狗狗，展示了 Python 在 IoT 領域的潛力。然而，提案可以更深入地探討技術細節，例如 ESP32 的具體應用、MicroPython 的程式碼範例，以及遇到的技術挑戰與解決方案。此外，可以更明確地說明這個專案對 Python 社群的價值，例如分享實用的程式碼或硬體設計。
-建議可以增加更多關於 MicroPython 在 ESP32 上的應用細節，例如如何使用特定的函式庫、如何處理硬體互動等。同時，可以分享一些程式碼片段，讓聽眾更容易理解你的實作方法。
-如果能更深入地探討技術細節，並明確說明專案的價值，這個提案會更具吸引力。</t>
+          <t>This proposal presents an interesting and unusual application of MicroPython on ESP32 for dog training. It highlights the challenges and learnings from a hobby project, including hardware integration and rapid prototyping limitations. While the topic is unique, the Python-specific technical depth could be increased. Consider elaborating on the MicroPython code used for logging, device control, and any specific libraries or techniques employed. The correlation between coding principles and hobby projects is a good point, but could be strengthened with concrete examples. The proposal could also benefit from a clearer demonstration of how Python is central to the project, rather than just a tool used for controlling hardware. To improve, focus on the Python aspects and provide more technical details about the implementation.</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1494,12 +1498,13 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>The proposal presents a Python tool for benchmarking local LLMs. While relevant, it lacks depth in Python-specific techniques and focuses more on the tool's impact. More emphasis on Python code and challenges would improve the proposal.</t>
+          <t>The proposal introduces `ollama-benchmark`, a tool for evaluating local LLM performance. It highlights its use in identifying and verifying a bug fix in Ollama and aims to educate attendees on building open-source tools. The tool collects hardware specs and throughput data to help users make informed decisions about hardware purchases.</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>This proposal discusses a tool built with Python (ollama-benchmark) to evaluate the performance of local LLMs (Ollama). While the topic of local LLMs is interesting, the proposal focuses more on the tool itself and its impact on the Ollama community rather than showcasing advanced Python techniques or innovative applications. The outline includes topics like folder structure, command-line parsing, and YML file usage, which are quite basic. To improve, the proposal could delve deeper into the Python code used for benchmarking, data analysis, or visualization. It could also explore how the tool leverages specific Python libraries for performance optimization or parallel processing. Highlighting the challenges faced during development and the solutions implemented using Python would also add value. The ethical considerations of collecting and displaying user hardware information are mentioned, which is a plus.</t>
+          <t xml:space="preserve">This proposal discusses the creation and usage of the `ollama-benchmark` tool for evaluating local LLM performance, particularly focusing on its role in identifying and verifying a bug fix in Ollama. The talk aims to educate attendees on building open-source tools and contributing to the community. While the tool itself seems valuable, the proposal needs to better highlight the Python aspects. The outline mentions using YML files and command-line parsing, but the connection to Python could be strengthened by elaborating on the Python libraries used and the challenges faced during development. To improve, the speaker should emphasize the Python code involved, the specific Python libraries used (e.g., for data processing, web scraping, or visualization), and the lessons learned in the Python development process. Also, the talk could benefit from a deeper dive into the data analysis techniques used to interpret the benchmark results. Without a stronger Python focus, it might be better suited for a more general AI/ML conference.
+</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1628,12 +1633,12 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Good topic on Python microservices on AWS Lambda. Suggest adding more concrete examples and elaborating on the tools used. Prerequisite might be too high.</t>
+          <t>This talk shares the practical implement of building Python microservices solution on AWS Lambda, including best practices and tuning methods. It leverages tools like Powertools for AWS Lambda and AWS Lambda Power Tuning.</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>This proposal focuses on using Python with AWS Lambda for serverless applications, which aligns well with PyCon's interest in practical Python applications. The talk includes best practices and tuning strategies, which are valuable for the audience. However, the proposal could benefit from more specific examples of the challenges faced and solutions implemented. Also, while Powertools and Power Tuning are mentioned, elaborating on how they are used in practice would enhance the technical depth. Consider adding a demo or case study to illustrate the concepts. The prerequisite seems a bit high, consider if it can be lowered to attract more audience.</t>
+          <t>This proposal focuses on building Python microservices on AWS Lambda, which is relevant to PyCon. It mentions practical implementation and tools like Powertools for AWS Lambda. However, the abstract and outline could be more specific about the challenges and solutions discussed. Detailing the 'best practices' and tuning methods would strengthen the proposal. The prerequisite seems a bit high, which might limit the audience.</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -1767,17 +1772,18 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>A well-structured talk on pivot tables in Pandas, targeting users familiar with Pandas but new to pivot tables. Could be improved by adding real-world use cases and performance considerations.</t>
+          <t>This talk will cover pivot tables in Pandas, explaining how to create them, their versatility, and advanced manipulation techniques. It targets those familiar with Pandas but new to pivot tables, promising practical examples and cool tricks.</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>This proposal clearly explains pivot tables in Pandas, a very useful tool for data analysis. The outline is well-structured and covers various aspects, including multi-indexes and datetime columns. It targets an audience familiar with Pandas but not pivot tables, which is a good niche. The talk promises practical examples and cool tricks, making it appealing. However, the proposal could benefit from mentioning specific real-world use cases or datasets where pivot tables shine. Adding a brief discussion of performance considerations for large datasets would also enhance the technical depth. Consider adding a section on how pivot tables can be used in conjunction with other Pandas functionalities for more complex analysis.</t>
+          <t>This proposal clearly outlines the benefits and practical applications of pivot tables in Pandas, targeting an audience familiar with Pandas but not necessarily with pivot tables. It promises to cover various aspects, from basic creation to advanced manipulation techniques like multi-indexes and stack/unstack. The outline is well-structured, and the objective is clearly defined. The proposal focuses specifically on Python and the Pandas library, making it highly relevant to PyCon. The speaker also promises to show cool tricks to use with pivot tables. This is a strong proposal.
+Potential improvements: While the outline is good, adding a specific example or two of the "cool tricks" would make the proposal even stronger.</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -1909,12 +1915,13 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>A deep dive into Python's import system, suitable for intermediate to advanced users. Covers finders, loaders, and the inner workings of the `import` statement. Could benefit from real-world examples and performance considerations.</t>
+          <t>This talk explains the inner workings of Python's import mechanism, including finders, loaders, and the `importlib` module. It targets intermediate to advanced Python users and aims to provide a deeper understanding of how modules are loaded and managed.</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>This proposal delves into the often-overlooked mechanics of Python's import system. It promises to cover a range of topics, from the basics of the `import` statement to more advanced concepts like custom finders and loaders. The outline is well-structured, and the objective clearly defines the target audience and expected takeaways. The talk seems well-suited for intermediate to advanced Python users who want a deeper understanding of the language's inner workings. The proposal could be strengthened by including specific examples of how custom finders/loaders can be used in real-world scenarios. Also, consider adding a brief mention of any potential performance implications of the import system.</t>
+          <t>This proposal delves into the often-overlooked mechanics of Python's import system. It promises to cover a range of topics, from the basics of the `import` statement to more advanced concepts like custom finders and loaders. The detailed description suggests a comprehensive exploration of the module loading process, which could be very insightful for intermediate to advanced Python users. The outline provides a clear structure for the talk. However, the proposal could benefit from including a specific example or use case where customizing finders or loaders would be beneficial. This would make the talk more practical and engaging.
+Vote: +1</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
@@ -2051,12 +2058,12 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Explores the intricacies of assignment in Python, suitable for experienced developers. Comprehensive outline and clear objectives. Strong focus on Python internals.</t>
+          <t>This talk explores the intricacies of assignment in Python, covering variable scopes, bytecodes, and descriptors. It aims to clarify the differences between assigning to a variable, an element of a list, and an attribute, targeting experienced Python developers.</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>This proposal dives deep into the mechanics of assignment in Python, covering variable scopes, bytecodes, and descriptors. It's a great topic for intermediate to advanced Python users. The outline is comprehensive and well-structured. The objective is clearly defined, targeting experienced Python developers. The talk promises to clarify the nuances between variable assignment, attribute assignment, and mutation. This proposal aligns well with PyCon's focus on in-depth Python knowledge. However, the abstract could be more concise and engaging.</t>
+          <t>This proposal offers a deep dive into Python's assignment mechanisms, covering variable scopes, bytecodes, and descriptors. It's highly relevant to PyCon, providing valuable insights for experienced Python developers. The outline is well-structured, and the objective clearly defines the target audience. The proposal could be strengthened by including specific examples or case studies to illustrate the concepts discussed. Consider adding a section on practical implications or potential pitfalls related to assignment in Python.</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
@@ -2168,12 +2175,12 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>The proposal focuses on the math behind SVMs, lacking Python-specific implementation details. Adding practical Python examples would improve its relevance to PyCon.</t>
+          <t>An introduction to Support Vector Machines and the math behind them. The proposal lacks specific details on how SVMs are implemented and used with Python.</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>This proposal introduces Support Vector Machines (SVMs) and the math behind them. While SVMs can be implemented in Python, the proposal seems to focus more on the mathematical concepts than the practical application or Python-specific implementation details. To be a stronger fit for PyCon, the presentation could benefit from including examples of how SVMs are used in Python, perhaps with libraries like scikit-learn, and discussing any Python-specific challenges or optimizations. Without this, it might be better suited for a more general machine learning conference.</t>
+          <t>This proposal introduces Support Vector Machines (SVMs) and the math behind them. While the topic itself is relevant to machine learning, the proposal doesn't explicitly mention the use of Python. To make it more suitable for PyCon, the presentation should include examples of how SVMs are implemented and used with Python libraries like scikit-learn. The presentation could also benefit from demonstrating practical applications of SVMs in Python-based projects. Without these Python-specific details, the proposal is only weakly related to the PyCon theme.</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
@@ -2299,12 +2306,12 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>Interesting topic but lacks Python-specific details. Needs more information on Python libraries and frameworks used for LLM interaction and data manipulation.</t>
+          <t>This proposal explores using LLMs and distillation to generate synthetic data for problem-solving. It lacks specific details on Python implementation and frameworks.</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>The proposal discusses using LLMs and distillation to create synthetic data. While interesting, the proposal lacks specific details on how Python is used in this process. To improve, the speaker should elaborate on the Python libraries and frameworks used for LLM interaction, data manipulation, and distillation. The current description is very general and needs more technical depth related to Python.</t>
+          <t>The proposal discusses using LLMs to create synthetic data for problem-solving, focusing on distillation techniques. While the topic is interesting, the proposal lacks specific details on the Python aspects and implementation. To improve, the speaker should elaborate on the Python libraries and frameworks used (e.g., TensorFlow, PyTorch) and provide concrete examples of how the synthetic data is generated and used within a Python environment. The outline and descriptions are repetitive and need to be more structured. Without more Python-specific details, the proposal is only weakly related to PyCon.</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
@@ -2426,12 +2433,12 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>Interesting topic but lacks a strong connection to Python. Needs to demonstrate Python usage for interacting with and analyzing LLMs.</t>
+          <t>The proposal explores Llama's ability to generate storylines and discusses its limitations in understanding contexts and metaphorical language. It lacks a clear connection to Python.</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>The proposal discusses using Llama for story generation and explores its limitations. While interesting, the connection to Python is weak. The proposal needs to explicitly demonstrate how Python is used (e.g., libraries for interacting with LLMs, data processing, or analysis of the generated stories). Without a stronger Python focus, it's more suitable for an AI conference. Consider adding details about the Python code used to interact with Llama and analyze its output.</t>
+          <t>The proposal discusses using Llama, a large language model, for story gaming and explores its limitations in understanding contexts and metaphorical language. While the topic of LLMs is interesting, the proposal lacks a clear connection to Python. It doesn't specify how Python is used in the process of testing or interacting with Llama. To make it suitable for PyCon, the proposal needs to emphasize the role of Python, such as using Python libraries for prompting, data analysis, or model evaluation. Without a stronger Python focus, it's more appropriate for an AI-focused conference. Consider adding details about Python code used for interacting with the LLM or analyzing its output. Also, the proposal seems to repeat the same content in different sections (abstract, detailed description, outline, objective).</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
@@ -2558,12 +2565,12 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>Interesting topic but lacks a strong Python focus. Needs to demonstrate Python's role in interacting with and testing the LLM. Content is repetitive.</t>
+          <t>This proposal explores the capabilities and limitations of the Llama language model in predicting the future, focusing on its understanding of context, math, and metaphorical language. It lacks a strong connection to Python.</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>The proposal discusses using Llama, a large language model, to predict the future and explores its limitations. While the topic is interesting, the connection to Python is weak. The proposal needs to explicitly demonstrate how Python is used to interact with and test the LLM. Without a stronger Python focus, it's more suitable for an AI conference. Consider adding details about Python libraries used for data processing, model interaction, or result analysis. Also, the proposal seems repetitive; ensure the content is concise and well-structured.</t>
+          <t>The proposal discusses using Llama, a large language model, to predict the future and explores its limitations in understanding contexts, verbal math, and metaphorical language. While the topic is interesting, the connection to Python is not strong. To be a better fit for PyCon, the proposal should emphasize the use of Python libraries or frameworks in the testing and analysis of Llama. For example, it could discuss using Python for data processing, model evaluation, or visualization of the results. Without a stronger Python focus, this proposal is more suitable for an AI or data science conference.</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
@@ -2690,12 +2697,12 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>The proposal offers a practical guide to using PyArrow with Pandas, covering file I/O, backend storage, and performance. It's relevant and well-structured, but could benefit from more specific examples and a discussion of potential challenges.</t>
+          <t>This talk introduces Apache Arrow and PyArrow to Pandas users, explaining how it can optimize their Pandas projects. It covers practical uses for reading/writing files and as a back-end storage system, highlighting efficiency gains compared to NumPy.</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>This proposal clearly addresses a relevant and important topic for Pandas users. The integration of PyArrow is a significant development, and the talk promises to provide practical guidance on how to leverage it. The outline is well-structured, covering essential aspects like file I/O, backend storage, and performance comparisons. The objective is well-defined, targeting Pandas users who are curious about PyArrow but lack practical knowledge. However, the proposal could benefit from more specific examples of complex operations where PyArrow shines or falls short. Also, elaborating on the challenges and solutions encountered during the integration process would add more depth. Consider adding a section on potential pitfalls or gotchas when using PyArrow with Pandas.</t>
+          <t>This proposal clearly explains the benefits of using PyArrow with Pandas, including faster CSV loading and memory efficiency. The outline is well-structured and covers practical use cases. It would be beneficial to include specific code examples demonstrating the performance improvements and memory savings. Also, mentioning potential drawbacks or limitations of PyArrow in certain scenarios would provide a more balanced perspective. Consider elaborating on the 'more complex things' section in the outline with concrete examples.</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
@@ -2830,17 +2837,17 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>The proposal effectively addresses a common Python development challenge by advocating for the use of the `logging` module over `print`. It offers a structured approach to learning `logging`, making it accessible to developers of varying experience levels.</t>
+          <t>This talk aims to teach Python developers how to effectively use the `logging` module instead of relying on `print` statements for debugging. It covers basic and advanced logging techniques, including configuration, formatting, filtering, and alternative logging libraries.</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>This proposal addresses a common pain point for Python developers: the overuse of `print` for debugging and the perceived complexity of the `logging` module. The talk promises to demystify `logging` and demonstrate its benefits, which aligns well with PyCon's goal of promoting best practices and improving Python development skills. The outline is well-structured, covering basic to more advanced aspects of `logging`. A potential improvement could be to include a real-world case study or a practical example where `logging` significantly improves debugging or monitoring compared to `print`.</t>
+          <t>This proposal addresses a common pain point for Python developers: the overuse of `print` for debugging and the perceived complexity of the `logging` module. The speaker clearly outlines the benefits of using `logging` and promises to demystify its configuration and usage. The talk covers a comprehensive range of topics, from basic configuration to advanced features like handlers, formatters, and filters. The inclusion of alternative loggers on PyPI is a nice touch. The outline is well-structured and the objectives are clearly defined. This proposal would be highly beneficial to Python developers of all levels, especially those looking to improve their debugging and logging practices. No specific improvements are necessary; the proposal is well-written and comprehensive.</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
@@ -2972,12 +2979,12 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>The proposal provides a detailed explanation of Python dictionary implementation, suitable for intermediate Python developers. It could benefit from more real-world examples and a broader comparison with other languages.</t>
+          <t>This talk explains the implementation of Python dictionaries (hash tables). It covers hash functions, collision handling (chaining, linear/quadratic probing), resizing, and Python 3.6 changes. The goal is to provide a deeper understanding of how dictionaries work internally.</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>This proposal offers a deep dive into the implementation of Python dictionaries, which is a core data structure. It covers hashing, collision handling, and the evolution of dictionaries in Python. The outline is well-structured, and the objective is clear: to demystify dictionaries for Python developers. The proposal could be strengthened by including specific examples of how understanding dictionary internals can lead to more efficient code in real-world scenarios. Also, consider adding a brief comparison with other hash table implementations in different languages to broaden the appeal.</t>
+          <t>This proposal offers a deep dive into the implementation of Python dictionaries, which is a core data structure. It covers hashing, collision handling, probing techniques, and even touches upon the changes introduced in Python 3.6. The talk aims to demystify dictionaries for Python developers, providing insights into their efficiency and design. The outline is well-structured, and the objective is clear. The proposal could be strengthened by including specific examples of how understanding dictionary internals can lead to better code optimization or more efficient data handling in real-world scenarios. Also, consider adding a brief comparison with other data structures to highlight the specific advantages of dictionaries.</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
@@ -3124,12 +3131,12 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>Interesting application of Python for language learning, but needs more depth in NLP techniques and practical impact. Could benefit from a more cohesive structure.</t>
+          <t>The proposal discusses using Python and NLP techniques to aid in learning Japanese, addressing challenges like character types and word segmentation using libraries like SudachiPy and jaconv.</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>This proposal introduces an interesting application of Python and NLP libraries (SudachiPy, jaconv, gTTS/Amazon Polly) for Japanese language learning. It covers key challenges like kanji readings and word segmentation. However, the proposal could benefit from a clearer demonstration of the practical impact and a deeper dive into the NLP techniques used. Consider adding specific examples of how these tools improve the learning process and perhaps comparing different NLP approaches. Also, explicitly state the Python version used and library version. The current outline is a bit fragmented; consolidating similar points would improve flow.</t>
+          <t>This proposal introduces how to use Python and NLP libraries to assist in learning Japanese, focusing on overcoming challenges like multiple character types and the absence of spaces between words. It covers practical applications of SudachiPy for morphological analysis and jaconv for character conversion. While the topic is interesting, its relevance to the core Python community might be limited. To enhance its appeal, the presentation could emphasize the innovative use of Python libraries and the specific coding techniques employed. Consider adding more details on the implementation and the challenges faced during development. Also, explicitly state the target audience's expected level of Python proficiency.</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
@@ -3254,12 +3261,12 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>Interesting topic but lacks a clear connection to Python and the PyCon audience. Needs to demonstrate how Python-related tools or practices can address the issues raised.</t>
+          <t>The proposal discusses the negative impacts of excessive meetings and the decline of written communication on focus, knowledge retention, and inclusivity. It advocates for asynchronous, written communication as a solution.</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>This proposal touches on interesting points about communication and knowledge retention in the modern workplace. However, its connection to Python and the PyCon audience is tenuous. While the problem is real, the talk doesn't seem to offer Python-specific solutions or insights. The outline is also quite abstract and lacks concrete examples or technical depth. To be suitable for PyCon, the speaker would need to clearly demonstrate how Python tools, practices, or communities can address the issues raised. For example, discussing how documentation generators, asynchronous communication libraries, or collaborative coding platforms can mitigate the negative effects of 'meeting-itis'.</t>
+          <t>The proposal raises an interesting point about the over-reliance on meetings and the decline of written communication. However, the connection to Python is weak. While the problem is relevant to software development in general, the proposal doesn't explain how Python or the Python community is specifically affected or how Python tools can be used to address the issue. The outline is also somewhat vague and doesn't suggest a strong technical focus. To improve, the proposal could explore how Python projects suffer from poor documentation or how asynchronous communication tools built with Python can help. Without a stronger Python connection, it's difficult to recommend this for PyCon.</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -3378,17 +3385,17 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>The proposal is a philosophical reflection on coding, lacking specific Python content and technical depth, making it a less suitable fit for PyCon TW without significant modifications.</t>
+          <t>A personal journey through software development paradigms, languages, and principles, aiming to inspire continuous improvement and explore advanced concepts. The connection to Python could be stronger.</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>This proposal focuses on the speaker's personal journey and philosophy of writing code, touching upon various programming paradigms and principles. While potentially inspiring, it lacks specific Python-related content and technical depth. The talk seems more suitable for a general software development audience rather than a Python-focused conference. To be a better fit for PyCon TW, the speaker should incorporate concrete Python examples, discuss Python-specific tools or frameworks, and demonstrate how these principles apply in the Python ecosystem.</t>
+          <t>This proposal discusses the speaker's personal journey in software development, touching upon various paradigms, languages, and principles. While the abstract mentions Python, the core focus seems to be on general software development concepts rather than specific Python techniques or libraries. The talk aims to inspire continuous improvement and explore advanced concepts like monads and functional programming. However, the connection to the PyCon audience and Python-specific content could be stronger. To improve, the speaker could incorporate more concrete Python examples and demonstrate how these concepts apply within the Python ecosystem. Without these improvements, the proposal might be better suited for a more general software development conference.</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>-0</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
@@ -3549,17 +3556,12 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>提案介紹了 LLM 在 RAG 知識管理和 LLM 服務化方面的應用，並涵蓋了相關的 Python 套件。建議增加更多程式碼範例和實際應用案例，並強調 Python 的核心作用。</t>
+          <t>本提案介紹大型語言模型在 RAG 知識管理和 LLM 服務化中的應用，涵蓋 sentence-transformer, pgvector, vLLM 和 Ollama 等 Python 套件。目標是幫助聽眾了解 LLM 應用程式開發，並激發創新。</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>這個提案涵蓋了大型語言模型（LLMs）在 RAG 知識管理和 LLM 服務化方面的實務應用，並介紹了相關的 Python 套件，例如 sentence-transformer、pgvector、vLLM 和 Ollama。內容與 PyCon 主題相關，且具有一定的技術深度。然而，可以更深入地探討這些套件的具體使用案例和最佳實踐，並強調 Python 在其中的作用。此外，可以考慮加入模型微調（Fine-Tune）的相關內容，以更全面地涵蓋 LLM 的應用。
-建議：
-1.  增加更多實際的程式碼範例，展示如何使用 Python 整合這些套件。
-2.  深入探討 RAG 和 LLM 服務化的具體應用場景，例如問答系統、聊天機器人等。
-3.  如果時間允許，可以簡要介紹模型微調的流程和方法。
-4.  在演講中強調 Python 在整個 LLM 應用流程中的核心作用。</t>
+          <t>這個提案涵蓋了大型語言模型（LLMs）在 RAG 知識管理和 LLM 服務化方面的實務應用，並介紹了相關的 Python 套件，如 sentence-transformer, pgvector, vLLM 和 Ollama。內容對於希望了解 LLM 應用程式開發的聽眾來說是有價值的。然而，提案可以更深入地探討這些套件的具體使用案例和技術細節，例如，展示如何使用這些套件解決實際問題，並提供更詳細的程式碼範例。此外，可以更明確地說明如何根據不同的應用場景選擇合適的 LLM 模型。建議在演講中加入更多的實作演示，以增強聽眾的參與感和學習效果。</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
@@ -3698,17 +3700,17 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>The proposal offers practical guidance on scaling Django apps with microservices, covering misconceptions, best practices, and real-world examples. More code examples and details on transition challenges would strengthen it.</t>
+          <t>This talk shares practical strategies and real-world examples on leveraging Django within a microservices architecture to enhance scalability and maintainability, addressing common misconceptions and highlighting best practices.</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>This proposal outlines a practical approach to scaling Django applications using a microservices architecture. It covers common misconceptions, best practices, and mistakes to avoid, offering valuable insights for developers. The inclusion of StackGuardian's architecture and Tirith provides a real-world example. To enhance the proposal, consider adding more specific code examples or performance benchmarks to demonstrate the benefits of the suggested practices. Also, elaborating on the challenges and solutions encountered during StackGuardian's transition to microservices would add depth.</t>
+          <t>This proposal outlines practical strategies for leveraging Django in a microservices architecture, which is highly relevant to PyCon. It addresses common misconceptions and highlights best practices, offering valuable insights for developers scaling Django applications. The agenda is well-structured, covering key aspects from monoliths to microservices and Django-specific considerations. The inclusion of StackGuardian's architecture and Tirith adds a practical dimension. To further enhance the proposal, consider adding more concrete examples of the mistakes to avoid and the best practices in action. Also, elaborating on the challenges and solutions encountered during StackGuardian's transition to microservices would be beneficial. The target audience is well-defined, and the learning objectives are clear. Overall, this is a strong proposal with potential for a highly informative and engaging talk.</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
@@ -3835,12 +3837,12 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>A good comparison of pandas, polars, and duckdb. Needs more specific examples and performance analysis. Well-suited for data professionals.</t>
+          <t>A comparison of pandas, polars, and duckdb for data wrangling in Python. The talk will cover the strengths, differences, and use cases of each library, providing guidance for data analysts, scientists, and engineers.</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>This proposal offers a good comparison of three popular data processing libraries in Python: pandas, polars, and duckdb. It outlines the strengths and weaknesses of each library and provides practical examples. However, the proposal could benefit from more specific examples and a deeper dive into the performance characteristics of each library. Consider adding benchmarks or real-world use cases to strengthen the presentation. Also, the outline includes 'import padnas as pd' which is a typo. Consider correcting this. The talk is well-suited for data analysts, scientists, and engineers who want to improve their data processing skills.</t>
+          <t>This proposal offers a good comparison of three popular Python data processing libraries: pandas, polars, and duckdb. It outlines the strengths and weaknesses of each, which is valuable for data professionals. The structure is clear and well-organized. To improve, the talk could benefit from more specific examples or case studies demonstrating the performance differences and trade-offs in real-world scenarios. Also, consider adding a section on how these libraries integrate with other Python tools in the data science ecosystem. The current outline is a bit high-level; adding more technical depth would be beneficial.</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -3953,12 +3955,12 @@
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>The proposal discusses building a recommendation system with Elasticsearch. It needs more focus on the Python aspects of the implementation to be a good fit for PyCon. More details on Python libraries and code examples are needed.</t>
+          <t>The proposal discusses building a recommendation system using Elasticsearch, highlighting its cost-effectiveness and power. It covers data collection, processing, model training, and real-time recommendations. The target audience includes data scientists, ML engineers, and business stakeholders.</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>This proposal outlines building a recommendation system using Elasticsearch. While Elasticsearch can be used with Python, the proposal doesn't emphasize the Python aspects sufficiently. The outline is clear, but the technical depth regarding Python integration (e.g., specific libraries used, data processing techniques with Python) needs to be strengthened. To be more suitable for PyCon, the presentation should focus more on the Python code and techniques used to interact with Elasticsearch for recommendation purposes. Consider adding details about Python libraries like `elasticsearch-py` and how they are used for querying and data manipulation. Also, discuss any Python-based data processing or feature engineering steps involved.</t>
+          <t>This proposal outlines building a recommendation system using Elasticsearch. While Elasticsearch can be used with Python, the proposal doesn't emphasize the Python aspects sufficiently. It focuses more on Elasticsearch functionalities. To improve, the speaker could highlight Python libraries used for data processing, model training (if applicable within Elasticsearch), or integration with applications. Mentioning specific Python tools and techniques would strengthen the proposal's relevance to PyCon. Without this, it leans more towards a general data science or Elasticsearch conference. The outline is clear, but lacks depth regarding Python's role.</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
@@ -4109,12 +4111,12 @@
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>Good introduction to using Python in robotics with ROS2. Clear outline and focus on accessibility for beginners. A demo and more details on Python libraries would improve the proposal.</t>
+          <t>This talk introduces using Python with ROS2 for robotics, aiming to demonstrate its accessibility for beginners. It covers ROS2 basics, controller connection with Pixhawk, and Python pub-sub code. A demo is planned to showcase the resulting code.</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>This proposal introduces using Python with ROS2 for robotics, which aligns well with PyCon's focus on Python. It highlights the accessibility of Python for beginners in robotics compared to C/C++. The outline is clear and covers essential aspects like ROS2 basics, Pixhawk controller connection, and Python pub-sub code. A live demo or video would significantly enhance the presentation. Consider elaborating on specific Python libraries used and potential challenges faced during development. Also, mentioning specific use cases or applications beyond a basic rover would increase the proposal's appeal.</t>
+          <t>This proposal introduces using Python with ROS2 for robotics, which aligns well with PyCon's focus on Python. It highlights the accessibility of Python for beginners in robotics compared to C/C++. The outline is clear and covers essential aspects like ROS2 basics, controller connection, and Python pub-sub code. A demo would significantly enhance the presentation. To improve, the proposal could benefit from more specific examples of Python code used for robot control and data processing, as well as a deeper dive into the challenges and solutions encountered when integrating Python with ROS2 and hardware like Pixhawk. Consider elaborating on the advantages and limitations of using Python in a robotics context, especially concerning performance and real-time constraints. Also, clarify the target audience's assumed level of Python and ROS knowledge.</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
@@ -4253,12 +4255,12 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>A well-structured proposal covering Python types and PEP 729, suitable for intermediate developers. More practical examples and use cases would enhance its appeal.</t>
+          <t>This talk explains the theory and practice behind Python types and PEP 729, covering type theory, gradual typing, and type checker comparisons. It aims to educate the audience on the new typing governance process and its implications.</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>This proposal provides a comprehensive overview of Python types, ranging from theoretical foundations to practical applications and the implications of PEP 729. The outline is well-structured, and the objectives are clearly defined. The talk aims to bridge the gap between type theory and its implementation in Python, which is valuable for intermediate Python developers. However, the proposal could benefit from more concrete examples of how PEP 729 impacts day-to-day Python development or specific use cases where the new governance process improves the type system. Highlighting the practical benefits and challenges of adopting PEP 729 would enhance the talk's appeal and relevance to the PyCon audience.</t>
+          <t>This proposal delves into the theoretical underpinnings of Python's type system and the motivations behind PEP 729. It aims to bridge the gap between type theory and practical implementation in CPython and various type checkers. The talk's structure is well-defined, covering type theory, gradual typing, and the specification process. However, the proposal could benefit from more concrete examples of how PEP 729 impacts developers and the Python ecosystem. Highlighting specific use cases or scenarios where the new governance process leads to tangible improvements would enhance its appeal. Also, while the outline mentions comparisons between type checkers, elaborating on the practical differences and trade-offs would be valuable. Consider adding a section on how developers can contribute to the type system under the new governance model.</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -4380,12 +4382,12 @@
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>提案旨在引導 Python 開發者閱讀 CPython 原始碼，了解底層實作。對於想深入了解 Python 運作原理的開發者很有幫助。建議增加實例和效能優化技巧。</t>
+          <t>本提案旨在引導 Python 開發者閱讀 CPython 原始碼，了解 Python 的運作原理，從而提高程式撰寫能力和信心。內容包括如何使用文字編輯器追蹤原始碼，以及探討物件、內建函數和常用資料結構的實現。</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>這個提案很有趣，能夠引導 Python 開發者深入了解 CPython 的底層實作。提案中提到使用文字編輯器追蹤原始碼，並以「不求甚解」的方式推敲資料結構和函數設計，這對於不熟悉 C 語言的 Python 開發者來說是一個很好的起點。建議可以更具體地展示如何使用 VSCode 或 Vim 進行原始碼追蹤，並提供一些實際的範例，例如追蹤 `list` 或 `dict` 的操作。此外，可以稍微提及一些常見的效能優化技巧，例如了解不同資料結構的時間複雜度。如果能加入一些實際案例，展示閱讀原始碼如何幫助解決實際問題，會更有說服力。</t>
+          <t>這個提案很有趣，能夠引導 Python 開發者深入了解 CPython 的底層實作。提案中提到使用文字編輯器追蹤原始碼，並探討物件、內建函數和常用資料結構，這對於提升開發者的技術深度很有幫助。建議可以加入一些實際的程式碼片段，展示如何閱讀和理解 CPython 原始碼，例如，可以選擇一個簡單的內建函數，逐步分析其原始碼實現。此外，可以更具體地說明閱讀原始碼如何幫助開發者寫出效能更好的程式。總體而言，這個提案具有相當的潛力，如果能夠加入更多實例和細節，將會更吸引人。</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
@@ -4520,12 +4522,12 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>A good overview of building a RAG application with Python, MongoDB, and Azure. Needs more focus on Python-specific implementation details and a less rushed demo outline.</t>
+          <t>This proposal demonstrates building a RAG application using Python, MongoDB Atlas Vector Search, and Azure services. It covers setting up MongoDB Atlas, Azure OpenAI, and deploying the application to Azure App Services. The target audience is Python developers who want to learn how to create RAG applications.</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>This proposal outlines a practical application of RAG using Python, MongoDB Atlas Vector Search, and Azure services. It targets Python developers who want to build RAG applications but lack the initial knowledge. The step-by-step demo is a strong point. However, the proposal could benefit from more details on the specific Python libraries used for interacting with MongoDB Atlas and Azure OpenAI, as well as the challenges encountered and solutions implemented during the RAG implementation. Also, the outline seems a bit rushed, with many setups crammed into a short demo time. Consider focusing on the core RAG implementation and streamlining the deployment aspects.</t>
+          <t>This proposal outlines a practical application of Python in building a RAG system using MongoDB Atlas Vector Search and Azure services. It targets Python developers who want to learn how to implement RAG applications. The step-by-step demo is a strong point. However, the proposal could benefit from more details on the specific Python libraries and code snippets used for integrating the different components. Also, elaborating on the challenges faced and solutions implemented during the development process would enhance the technical depth. Consider adding more details on how the Azure OpenAI service is integrated with MongoDB Atlas Vector Search using Python code. Also, consider focusing more on the Python aspects of the integration, rather than just describing the services themselves. This would make it more relevant to the PyCon audience.</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
@@ -4685,12 +4687,12 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>The proposal is relevant to the application of GAI in finance but lacks sufficient technical details about the Python technologies used. Adding more specifics about Python libraries and implementation details would improve its suitability for PyCon.</t>
+          <t>The proposal explores the use of Generative AI in the financial sector, covering applications, challenges, and the architecture of 玉山銀行's GENIE platform. It discusses key considerations like data privacy, budget management, and internal promotion strategies.</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>This proposal discusses the application of Generative AI (GAI) in the financial industry, which is a relevant and timely topic. It covers various aspects, including challenges, implementation, and management, and provides real-world examples from E.SUN Bank. The outline is well-structured, covering introduction, applications, issues, backend, and promotion. However, the proposal could benefit from a deeper dive into the specific Python technologies and frameworks used in developing and deploying these GAI solutions. For example, mentioning specific libraries used for data analysis, model deployment, or API integration would enhance the technical depth. Also, elaborating on the DLP mechanism and load balancing strategies with technical details would be beneficial. To improve the proposal, consider adding more technical details about the Python-related aspects of the GAI implementation. This would make it more appealing to the PyCon audience.</t>
+          <t>This proposal discusses the application of Generative AI (GAI) in the financial industry, focusing on challenges, implementation, and management. It covers various aspects, including GAI applications, potential issues, and the architecture of a GAI platform (GENIE). The proposal could be strengthened by providing more specific details on the Python technologies used in the development and deployment of GENIE, such as the frameworks, libraries, and tools employed. Additionally, elaborating on the data security and privacy measures implemented would enhance the proposal's relevance to the PyCon audience. Consider adding more technical depth regarding the implementation of DLP and load balancing. Also, while the 玉山銀行案例 is interesting, more focus on the Python aspects would be beneficial. The outline is well-structured and covers a range of relevant topics.</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
@@ -4813,12 +4815,12 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>提案展示了利用 LangChain 和 FastAPI 實現 LLM 數位孿生系統的方法，並分享了開源框架。建議更深入探討技術細節和提供實際應用案例。</t>
+          <t>本提案介紹如何利用 LangChain 與 FastAPI 整合開發 LLM 數位孿生系統，並分享開源框架 LLMTwins。透過 Google Sheet 設定提示工程，簡化資料清洗與向量化過程，降低開發門檻，並提供實際案例。</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>這個提案結合了 LangChain、FastAPI 和 LLM，展示了如何快速開發數位孿生系統，並整合第三方 API。講者分享的開源框架能幫助 Python 開發者更容易地進行提示工程，降低了 LLM 應用的門檻。然而，提案可以更深入地探討框架的技術細節，例如 LangChain Agent 的具體配置和 RAG 工具的向量化方法。此外，可以更詳細地說明數位孿生專案的實際應用，並提供實驗數據或性能指標，以增強說服力。</t>
+          <t>這個提案結合了 LangChain、FastAPI 和 LLM，展示了如何快速開發數位孿生系統，並整合第三方 API。講者分享的開源框架能幫助 Python 開發者簡化提示工程的流程，降低 LLM 專案的開發門檻。提案中提到的實際案例（如數位香菇寮）有助於聽眾理解技術的應用場景。建議可以更深入探討 LangChain Agent 和 RAG 工具的具體設定與調整方法，以及在不同 LLM 模型間切換時可能遇到的問題與解決方案。</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
@@ -4940,12 +4942,12 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>Good overview of concurrency in Python with practical examples. Suggest adding more code examples, performance trade-offs, and debugging techniques.</t>
+          <t>An introduction to concurrency and parallelism in Python using threads, processes, and coroutines. The talk includes real-world scenarios, challenges, and solutions for handling race conditions. Aims to provide Python developers with a clear understanding of these concepts.</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>This proposal provides a good overview of concurrency and parallelism in Python, covering threads, processes, and coroutines. The inclusion of practical scenarios and challenges faced is a strong point. To enhance the proposal, consider adding more specific examples of how these concurrency methods are implemented in Python, including code snippets. Also, elaborate on the performance trade-offs between threads, processes, and coroutines in different scenarios. Addressing the Python GIL and its impact on multithreading performance is crucial. The outline is well-structured, but ensure sufficient time is allocated to each section, especially the practical examples and Q&amp;A. Consider adding a section on debugging concurrent code.</t>
+          <t>This proposal provides a good introduction to concurrency and parallelism in Python, covering threads, processes, and coroutines. The inclusion of real-world scenarios and challenges faced is a strong point. To improve, the talk could delve deeper into the practical implementation details of each approach, including code examples and performance comparisons. Also, elaborating on specific strategies for handling race conditions beyond a general mention would be beneficial. Consider adding more details on how asyncio is used in practice. The outline is clear and well-structured. The objective is well-defined and addresses a common need for Python developers. Overall, this is a promising proposal that could be a valuable addition to PyCon TW.</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
@@ -5102,12 +5104,12 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>The proposal is relevant to PyCon, focusing on using Python (KerasNLP) for LLM fine-tuning with LoRA. More details on implementation challenges and quantitative results would improve it.</t>
+          <t>This proposal introduces how to fine-tune Large Language Models (LLMs) with LoRA using KerasNLP. It covers loading pre-trained GPT-2 models, explaining LoRA, and comparing fine-tuned models. The talk aims to help developers understand the end-to-end process of LLM fine-tuning with KerasNLP.</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>This proposal focuses on fine-tuning LLMs using KerasNLP and LoRA, which is relevant to the application of Python in modern NLP. The outline is well-structured, covering the basics of GPT-2 fine-tuning and then diving into LoRA. A potential improvement would be to include more specific examples of the dataset used and the challenges encountered during fine-tuning. Also, quantifying the parameter efficiency gains with LoRA would strengthen the proposal.</t>
+          <t>This proposal focuses on fine-tuning LLMs using KerasNLP and LoRA, which is relevant to the application of Python in modern NLP. It provides a practical guide for developers to customize LLMs in a parameter-efficient way. The outline is clear and covers the key steps, including loading pre-trained models, explaining LoRA, and comparing the performance. The target audience is well-defined. However, the proposal could benefit from more details on the specific datasets used for fine-tuning and a deeper discussion of the challenges encountered during the process. Also, elaborating on the practical applications or use cases of the fine-tuned models would enhance the proposal's appeal. Consider adding more concrete examples or experimental results to strengthen the claims.</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
@@ -5246,12 +5248,12 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>Good overview of chatbot development with fine-tuned GPT. Suggest adding more Python-specific details and expanding on the challenges and solutions encountered during fine-tuning.</t>
+          <t>This talk introduces chatbot development using fine-tuned GPT models, covering the development workflow, implementation practices, and evaluation metrics. It aims to provide beginners with the knowledge to create their own chatbots.</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>This proposal outlines a practical guide to chatbot development using fine-tuned GPT models, which aligns well with the interests of many PyCon attendees. The inclusion of a live demo and a step-by-step guide is a strong point. However, the proposal could benefit from more specific details on the Python libraries and frameworks used for chatbot development and fine-tuning. Also, elaborating on the challenges encountered during the fine-tuning process and how they were overcome would add more depth. Consider adding more details on how to evaluate the chatbot using Python tools. The current outline is a bit brief; expanding on each section would be beneficial.</t>
+          <t>This proposal provides a good overview of chatbot development using fine-tuned GPT models. It's well-structured and aims to equip beginners with the necessary knowledge. The inclusion of a live demo is a strong point. However, the proposal could benefit from more specific details on the Python libraries and frameworks used for chatbot development and fine-tuning. Also, elaborating on the challenges encountered during the fine-tuning process and how they were addressed would add more depth. Consider adding more practical examples and code snippets to enhance the learning experience. The current outline seems a bit high-level; providing more concrete examples would be beneficial.</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
@@ -5383,12 +5385,13 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>Good introduction to RAG and LangChain. Needs more technical depth and focus on Python aspects. Consider adding more details on challenges and solutions, and specific Python libraries used.</t>
+          <t>This talk introduces RAG applications using LangChain, covering architecture, components, and a live demo. It targets Python developers interested in improving LLM answer quality. The proposal could benefit from more technical depth and practical details.</t>
         </is>
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>This proposal introduces RAG and LangChain, which are relevant to the application of Python in the field of LLMs. The outline is clear and includes a live demo, which is a plus. However, the proposal could benefit from more details on the specific challenges and solutions encountered when building RAG applications with LangChain. Also, it would be good to mention the specific Python libraries used within LangChain for different RAG components (e.g., vector databases). Consider adding more technical depth and focusing on the Python aspects of LangChain. The current proposal is a good introduction, but needs more technical details to be a strong accept.</t>
+          <t>This proposal introduces Retrieval Augmented Generation (RAG) applications using LangChain, a popular framework for LLM-powered applications. The talk covers the architecture and components of RAG with LangChain, including chunking, embeddings, and vector search, culminating in a live demo. The proposal clearly outlines the talk's structure and objectives, targeting Python developers interested in LLMs. While the topic is relevant and timely, the proposal could benefit from more specific details on the challenges and solutions encountered when building RAG applications with LangChain. For example, discussing specific techniques for optimizing vector search or handling different data sources would enhance the technical depth. The live demo is a great addition, but the proposal could elaborate on what the demo will showcase and what attendees will learn from it. Consider adding more details on error handling, scalability, or specific use cases to increase the practical value. Also, consider adding more details about the python packages used in the demo.
+Vote: +0</t>
         </is>
       </c>
       <c r="W36" t="inlineStr">
@@ -5517,12 +5520,12 @@
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>Good introduction to AWS CDK with Python for IaC. Needs more technical depth and specific Python examples.</t>
+          <t>The proposal discusses using Python CDK on AWS for infrastructure automation, focusing on improving efficiency and reducing human errors. It covers the benefits of IaC and aims to provide a practical introduction to deploying infrastructure using Python.</t>
         </is>
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>This proposal introduces AWS CDK with Python, which is relevant to PyCon. It highlights the benefits of IaC and automation. However, the proposal could benefit from more specific examples of how Python is used within the CDK framework and the challenges faced/solved. The outline is a bit high-level; consider adding more technical depth to the demo and real-world use cases.</t>
+          <t>This proposal introduces AWS CDK with Python, which is relevant to PyCon. It highlights the benefits of using Python for infrastructure automation and aims to provide a practical introduction to the topic. The outline is clear and covers key aspects of CDK. However, the proposal could benefit from more specific examples of how Python is used within CDK to solve particular infrastructure challenges. Detailing the types of reusable components and the specific best practices would also strengthen the proposal. Consider adding more technical depth to the demo and real-world use cases to make it more appealing to the PyCon audience.</t>
         </is>
       </c>
       <c r="W37" t="inlineStr">
@@ -5678,12 +5681,12 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>提案涵蓋 Python 在餐飲 POS 系統中的應用，內容廣泛但缺乏深度。建議增加實作細節和案例研究，以提升技術深度和實用性。</t>
+          <t>分享在餐飲 POS 系統公司使用 Python 的實戰經驗，涵蓋技術選型、挑戰、最佳實踐以及 AI 的影響。內容廣泛，對 Python 後端開發者具有參考價值。</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>這個提案描述了在餐飲 POS 系統公司使用 Python 的實戰經驗，涵蓋了技術選型、挑戰、最佳實踐以及 AI 的影響。內容廣泛，從 Web 框架到資料庫，再到 CI/CD 和監控，展現了 Python 在企業應用中的多個方面。然而，提案可以更具體地展示 Python 如何解決特定問題，例如，提供程式碼範例或更深入的技術細節。此外，AI 在 Python 開發環境中的應用可以更深入地探討，例如，展示 AI 如何輔助程式碼生成、測試或除錯。建議在演講中加入更多案例研究和實作細節，以增強聽眾的參與度和學習效果。</t>
+          <t>這個提案分享了在餐飲 POS 系統公司使用 Python 的實戰經驗，涵蓋了技術選型、挑戰、最佳實踐以及 AI 的影響。內容廣泛，從 Web 框架到資料庫，再到 CI/CD 和監控，對於 Python 後端開發者來說具有一定的參考價值。建議可以更深入地探討特定技術挑戰的解決方案，例如資料庫擴展或性能優化，並提供更具體的程式碼範例。此外，可以更明確地說明 AI 如何實際改善 Python 開發環境，例如自動程式碼生成或錯誤檢測。</t>
         </is>
       </c>
       <c r="W38" t="inlineStr">
@@ -5814,12 +5817,12 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>Good introduction to LangChain for Text-to-SQL. Suggest adding more Python code examples and elaborating on the challenges and solutions.</t>
+          <t>This talk explores using LangChain to query structured data with an AI agent. It includes a live demo of LangChain's SQL agent, showcasing its ability to generate SQL queries from text and answer questions based on the query results. The target audience is Python developers interested in Generative AI.</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>This proposal introduces LangChain for Text-to-SQL, which is relevant to Python developers interested in Generative AI. The live demo is a plus. However, the proposal could benefit from more details on the specific Python code used with LangChain and the challenges encountered during implementation. Also, it would be helpful to elaborate on how LangChain addresses the limitations of LLMs in the context of SQL queries beyond just mentioning "hallucinations".</t>
+          <t>This proposal introduces LangChain for querying structured data, which is relevant to Python developers interested in Generative AI. The live demo is a great way to showcase the tool's capabilities. However, the proposal could benefit from more details on the specific Python libraries used within LangChain and the challenges encountered during implementation. Also, it would be helpful to elaborate on how LangChain addresses the limitations of Text-to-SQL, beyond just reducing hallucinations. Consider adding more technical depth regarding the vector store and the selection of "golden sample" queries. The outline is clear and well-structured.</t>
         </is>
       </c>
       <c r="W39" t="inlineStr">
@@ -5966,12 +5969,12 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>提案詳細介紹了如何使用 FastAPI 和 Grafana Stack 增強 Python 服務的可觀測性，涵蓋 Logs、Metrics 和 Traces，並提供實際案例。內容對開發和運維人員都有價值。</t>
+          <t>本提案介紹如何使用 FastAPI 和 Grafana Stack 強化 Python 服務的可觀測性，涵蓋 Logs、Metrics 和 Traces，並介紹 OpenTelemetry、Prometheus 等工具。目標是幫助開發和運維人員快速追蹤 Bug 和定位線上問題。</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>這個提案很好地結合了 FastAPI 和 Grafana Stack，展示了如何增強 Python 服務的可觀測性。內容涵蓋了 Logs、Metrics 和 Traces 三個方面，並介紹了 OpenTelemetry、Prometheus、Loki、Tempo 等工具的使用。提案大綱清晰，目標受眾明確，既適合開發人員也適合運維人員。如果能更深入地探討在實際生產環境中遇到的挑戰和解決方案，會更有價值。建議可以增加一些關於可觀測性資料的安全性考量。</t>
+          <t>這個提案很好地結合了 FastAPI 和 Grafana Stack，展示了如何強化 Python 服務的可觀測性。內容涵蓋了 Logs、Metrics 和 Traces 三個方面，並介紹了 OpenTelemetry、Prometheus、Loki、Tempo 等工具的使用。提案大綱清晰，目標受眾明確，既適合開發人員也適合運維人員。建議可以更深入地探討在實際生產環境中遇到的挑戰和解決方案，例如大規模服務的可觀測性策略、資料採樣和過濾等。此外，如果能提供更多實際案例和實驗數據，將會更有說服力。</t>
         </is>
       </c>
       <c r="W40" t="inlineStr">
@@ -6124,17 +6127,18 @@
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>Addresses memory profiling in PySpark with Memray, a relevant topic. Could benefit from more practical examples and deeper insights into optimization techniques.</t>
+          <t>This talk focuses on using Memray to effectively memory profile distributed PySpark code, especially when dealing with native extensions. It compares Memray with the built-in PySpark memory profiler and provides a deep dive into challenging memory profiling cases, including examples with Apache Arrow and Polars. The talk aims to help users scale up their data analysis code and solve memory usage issues in distributed computations.</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>This proposal focuses on memory profiling of distributed PySpark code using Memray, which is highly relevant to PyCon. It addresses a challenging aspect of PySpark development, especially when dealing with native extensions. The comparison with the built-in PySpark memory profiler is valuable. The outline is well-structured, and the objective is clear.  It would be beneficial to include more details on specific memory profiling techniques and optimization strategies. Also, elaborating on the 'best practices' for converting pandas to PySpark code would enhance the practical value. Consider adding more real-world examples or case studies to strengthen the presentation.</t>
+          <t>This proposal addresses a very practical and challenging problem: memory profiling in distributed PySpark code, especially when native extensions are involved. The talk clearly outlines the motivation, the tools (Memray), and the target audience. The comparison with the built-in PySpark memory profiler is a good touch. The outline is well-structured and promises a deep dive into real-world scenarios. The focus on using Memray to profile memory usage in challenging distributed situations is valuable. The inclusion of examples with Apache Arrow and Polars further strengthens the proposal. However, the proposal could benefit from more concrete examples of the "challenging data processing scenarios" mentioned in the abstract. Also, while Memray is introduced, more emphasis on its specific features and how they address the challenges of profiling in a distributed environment would be beneficial. Finally, elaborating on the "best practices for converting pandas to PySpark code" would add more value.
+Vote: +1 because it is highly relevant to PyCon, addresses a practical problem, and offers a solution using a relatively new tool.</t>
         </is>
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="X41" t="inlineStr">
@@ -6300,12 +6304,12 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>提案介紹使用 GAI 技術的資訊助手平台，具備一定實用性。建議加強 Python 在資料處理和工具整合方面的技術細節，並分享實作經驗。</t>
+          <t>本提案介紹 oh my gai 平台，該平台使用 GAI 技術自動蒐集、分類、評分和摘要 GAI 相關資訊，幫助使用者更有效率地掌握 GAI 技術的發展。平台使用 ChatPaper 摘要論文，並使用 RankGPT 對文章評分。</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>這個提案介紹了一個使用 GAI 技術來蒐集、分類、評分和摘要資訊的平台，對於想要了解 GAI 最新發展的聽眾來說，具有一定的吸引力。提案中提到了使用 Python 進行資料蒐集和處理，並使用了 ChatPaper 和 RankGPT 等工具，但 Python 在整個流程中所扮演的角色可以更明確地強調。建議可以更深入地探討如何使用 Python 整合這些工具，以及如何使用 Python 進行資料清洗、轉換和分析。此外，可以分享更多在實作過程中遇到的挑戰和解決方案，以增加技術深度。Demo 部分可以更具體地展示平台的功能和使用方法。</t>
+          <t>這個提案介紹了一個使用 GAI 技術來蒐集、分類、評分和摘要 GAI 相關資訊的平台。優點是主題與當前熱門的 GAI 趨勢相關，並展示了如何利用 Python 和 GAI 工具（如 ChatPaper 和 RankGPT）來解決資訊過載的問題。缺點是技術深度可能需要加強，例如可以更深入地探討如何優化 prompt 工程以提高分類和評分的準確性，以及如何處理 GAI 模型可能產生的偏差。建議在 Demo 環節展示更多實際案例，並分享在構建平台過程中遇到的挑戰和解決方案。可以考慮加入更多關於如何使用 Python 進行資料處理和模型整合的細節。</t>
         </is>
       </c>
       <c r="W42" t="inlineStr">
@@ -6483,13 +6487,12 @@
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>提案介紹了一個基於 Python 的跨平台自動化測試框架，解決了跨平台和跨時代環境整合的難題。建議增加實際應用案例和程式碼範例，以增強說服力。</t>
+          <t>本提案介紹一個基於 Python 的跨平台自動化測試框架，旨在解決跨平台和跨時代環境整合測試的挑戰。該框架支援多種作業系統，並能高效重用測試程式碼，實現測試流程的平行化。與 CI Runner 和 Robot Framework 相比，該框架在運行環境、長時間測試和靈活性方面具有優勢。</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>這個提案介紹了一個基於 Python 的跨平台自動化測試框架，解決了軟體測試中跨平台和跨時代環境整合的難題。提案詳細描述了框架的設計、優勢以及與其他工具（如 CI Runner、Robot Framework、PyTest）的比較。優點是問題意識明確，解決方案也具有一定的實用價值。建議可以更深入地探討框架在實際應用中的案例，例如具體的測試案例、性能數據等，以增強說服力。此外，可以更詳細地介紹如何利用 Python 的特性來實現跨平台兼容性，例如使用哪些特定的 Python 庫或技術。
-這個提案適合對跨平台測試和自動化測試感興趣的 Python 開發者和測試工程師。如果能夠在演講中展示更多實際的程式碼範例和測試結果，將會更具吸引力。</t>
+          <t>這個提案介紹了一個基於 Python 的跨平台自動化測試框架，解決了跨平台和跨時代環境整合測試的挑戰。提案詳細描述了框架的設計、優勢以及與其他工具（如 CI Runner、Robot Framework、PyTest）的比較。優點是解決了實際痛點，並提供了開源專案連結。建議可以更深入地探討框架在不同作業系統上的具體實作細節，以及如何利用 Python 的特性來優化測試流程。此外，可以考慮提供更多實際案例或實驗數據，以增強提案的說服力。</t>
         </is>
       </c>
       <c r="W43" t="inlineStr">
@@ -6617,12 +6620,12 @@
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>Interesting topic but needs more focus on Python aspects and practical applications. Add code examples and real-world use cases.</t>
+          <t>The proposal introduces Parametric Spectral Clustering (PSC), a novel solution addressing limitations of spectral clustering, and its Python library. It covers principles, advantages, and experimental results.</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>This proposal introduces Parametric Spectral Clustering (PSC) and its Python library. While the topic itself is interesting, the proposal needs to better highlight the Python-specific aspects and practical applications within the Python ecosystem. The outline is clear, but the presentation should emphasize the library's usage and benefits for Python developers. Consider adding code examples and real-world use cases to increase its relevance to the PyCon audience.</t>
+          <t>This proposal introduces Parametric Spectral Clustering (PSC) and its Python library, which addresses limitations of traditional spectral clustering. The presentation covers the principles, advantages, and experimental results of PSC. While the topic is relevant to data science, its connection to core Python aspects could be strengthened. Consider emphasizing the Python library's implementation details, API design, and how it leverages specific Python features for performance or usability. Adding practical examples of how the library can be used in real-world Python projects would also enhance the proposal. The outline is clear and well-structured.</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
@@ -6780,12 +6783,12 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>A good overview of Python dashboarding tools with a practical comparison. Consider adding code examples and elaborating on challenges faced during dashboard creation.</t>
+          <t>This talk compares Python dashboarding tools (Dash, Panel, Voila, Streamlit) using a dataset of visitors to Taiwan. It covers framework strengths, weaknesses, and integration with AI/big data. The target audience includes data analysts and developers seeking the best tool for their needs.</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>This proposal offers a good overview of popular Python dashboarding tools. It clearly outlines the strengths and weaknesses of each framework (Dash, Panel, Voila, Streamlit) and provides a practical comparison. The use of a visitor dataset from Taiwan adds a local context. To enhance the proposal, consider including specific code snippets or examples demonstrating the integration of these frameworks with AI/Big Data tools. Also, elaborating on the challenges and solutions encountered during the dashboard creation process would add more depth. The target audience is well-defined.</t>
+          <t>This proposal provides a good overview of popular Python dashboarding tools. It clearly outlines the strengths and weaknesses of each framework (Dash, Panel, Voila, Streamlit) and offers a practical comparison. The use of a real-world dataset (visitors to Taiwan) enhances the proposal's appeal. To improve, the talk could include a brief demo or code snippet for each framework to showcase its ease of use and capabilities. Additionally, elaborating on specific use cases or scenarios where each framework excels would be beneficial. Consider adding a section on deployment strategies for these dashboards. The outline is well-structured and the objectives are clearly defined.</t>
         </is>
       </c>
       <c r="W45" t="inlineStr">
@@ -6931,12 +6934,13 @@
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>提案結合天文學、Python和遊戲，具備創新性。建議加強Ren'Py的技術細節描述，並提供更多程式碼範例。</t>
+          <t>本提案介紹如何使用ChatGPT和Ren'Py遊戲引擎創建一個天文學學習遊戲《獵星者旅店》。講者將分享如何利用Astroquery套件獲取天文資料，並將ChatGPT整合到Ren'Py遊戲中，以提供互動式學習體驗。</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>這個提案結合了天文學、Python和遊戲，是一個有趣的嘗試。利用ChatGPT和Ren'Py來推廣天文知識，具有一定的創新性。然而，提案中關於Ren'Py的技術細節描述較少，建議可以更深入地探討在Ren'Py中使用Python套件和API的具體方法，例如如何解決相容性問題、如何優化效能等。此外，可以考慮加入更多實際的程式碼範例，讓聽眾更容易上手。如果能更聚焦在Ren'Py的技術實作，並減少ChatGPT的篇幅，會更符合PyCon的主題。</t>
+          <t xml:space="preserve">這個提案結合了天文學、Python和遊戲開發，是一個有趣的結合。利用ChatGPT和Ren'Py來創建互動式學習體驗，有潛力吸引對天文學和Python有興趣的聽眾。然而，提案需要更深入地探討Ren'Py的技術細節，例如如何在Ren'Py中安裝和使用Astroquery套件，以及如何解決實際開發中遇到的問題。此外，可以更明確地說明聽眾將從這個演講中學到哪些具體的Python技能和天文知識。建議增加更多關於Ren'Py和Astroquery的程式碼範例，並更詳細地說明如何將ChatGPT整合到Ren'Py遊戲中。
+</t>
         </is>
       </c>
       <c r="W46" t="inlineStr">
@@ -7106,12 +7110,12 @@
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>提案主題與 ESG 相關，但 Python 技術深度需加強。建議增加 Python 在資料介接、計算和系統架構中的應用細節。</t>
+          <t>本提案介紹講者開發的碳排放量管理系統，該系統基於 ISO-14064、ISO-14067 標準和 CBAM 計算方法，旨在幫助製造業量化和管理碳排放量。講者將分享與水五金、手工具和紡織纖維廠商合作的經驗，並介紹如何使用 Python 介接資料和實作計算。</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>這個提案介紹了使用 Python 開發碳排放量計算系統的經驗，並結合了 CBAM、ISO-14064 和 ISO-14067 等標準。優點是主題與當前熱門的 ESG 議題相關，並分享了實際導入案例。缺點是技術深度可能不足，需要更詳細地介紹 Python 在資料介接、計算和系統架構中的具體應用。建議加強 Python 相關技術細節的描述，例如使用的框架、函式庫以及解決方案。</t>
+          <t>這個提案介紹了使用 Python 開發碳排放量計算系統的經驗，並結合了 CBAM、ISO-14064 和 ISO-14067 等標準。優點是主題與當前熱門的 ESG 議題相關，並分享了實際案例。缺點是技術深度可能不足，需要更詳細地介紹 Python 在資料介接、計算和系統架構中的具體應用。建議增加 Python 程式碼範例，並深入探討技術挑戰與解決方案。</t>
         </is>
       </c>
       <c r="W47" t="inlineStr">
@@ -7239,12 +7243,12 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>Interesting concept combining Blender and Python for data visualization. Needs more technical depth and concrete examples to be a strong fit for PyCon.</t>
+          <t>This talk explores combining Blender's 3D animation with Python's graphing libraries for data storytelling. Attendees will learn to create immersive 3D models and integrate 2D plots for presenting data insights in education and professional projects.</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>This proposal presents an interesting intersection of Blender's 3D capabilities and Python's data visualization libraries. It has the potential to offer a novel approach to data storytelling. However, the proposal could benefit from more concrete examples of how the Python libraries are integrated with Blender, and a deeper dive into the technical challenges and solutions involved. The outline is clear, but the time allocated to each section seems a bit short, especially for demonstrating the integration of 2D plots into 3D models. To improve, the speaker should provide more specific code snippets or examples of how to use Blender's Python API to achieve the desired results. Also, elaborating on the 'real-world example' would enhance the proposal's appeal. Consider expanding the section on animating the visualizations to showcase more advanced techniques.</t>
+          <t>This proposal presents an interesting intersection of Blender's 3D capabilities and Python's data visualization libraries. The idea of creating dynamic data storytelling through 3D models enhanced with 2D plots is innovative and could be appealing to educators and data enthusiasts. However, the proposal needs to provide more concrete details on the Python code involved, specifically how data is transferred between Python and Blender, and how the 2D plots are embedded and animated within Blender. The outline is a bit high-level; adding more technical depth would strengthen the proposal. Consider including specific examples of Python code snippets or demonstrating the Blender Python API usage. Also, elaborating on the 'real-world example' in the storytelling section would enhance the practical value. Without more detail, it's hard to assess the technical depth for a PyCon audience.</t>
         </is>
       </c>
       <c r="W48" t="inlineStr">
@@ -7374,12 +7378,12 @@
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>提案將行銷和專案管理應用於 Python 學習，但 Python 技術深度不足。建議加強技術細節和實作案例的分享。</t>
+          <t>講者分享如何運用社群行銷和專案管理方法來學習 Python，包含召開讀書會、使用專案管理工具等。Python 技術深度較淺，建議加強實作案例和程式碼展示。</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>這個提案很有趣，將文組的行銷和專案管理技能應用於 Python 學習。然而，提案中 Python 的技術深度略顯不足，更多著重於學習方法和工具的使用。建議可以更深入地分享在實際 coding 過程中遇到的技術挑戰和解決方案，例如具體的 bug 案例、使用的 Python 庫和技巧等。此外，可以更明確地展示 Python 實作成果，例如一個小型的 Python 專案或程式碼片段。Live demo 可以展示實際的 coding 過程或專案成果，增加聽眾的參與感。</t>
+          <t>這個提案描述了文組背景的講者如何運用社群行銷和專案管理方法來學習 Python。雖然分享了學習方法和工具，但 Python 技術深度不足，實作成果也較為基礎。建議可以更深入地展示 Python 程式碼範例，並分享解決實際 coding 問題的經驗。此外，可以更明確地說明如何將 Scrum 專案管理應用於 Python 學習，例如如何拆解學習任務、追蹤進度等。可以考慮將重點放在展示實際的 Python 專案和程式碼，並分享在學習過程中遇到的挑戰和解決方案。</t>
         </is>
       </c>
       <c r="W49" t="inlineStr">
@@ -7528,12 +7532,12 @@
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>提案主題新穎，結合 LLM/RAG 技術於 ESG 領域。建議加強技術細節、benchmark 數據呈現，並多分享實際案例。</t>
+          <t>本提案介紹如何使用 LLM 和 RAG 技術，結合 Python 套件（如 LangChain、LlamaIndex），打造一站式 ESG 資訊查詢及報告生成平台。目標受眾包括技術開發者、ESG 專業人士和企業決策者。</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>這個提案結合了 LLM 和 RAG 技術於 ESG 領域，是一個相當熱門且具潛力的主題。提案中提到了幾個流行的 LLM 模型和 Python 套件，例如 LangChain 和 LlamaIndex，顯示講者對此領域有一定的了解。然而，提案可以更深入地探討這些工具的具體應用方式，以及在 ESG 報告生成過程中遇到的挑戰和解決方案。此外，benchmark 的評估標準和數據可以更詳細地呈現，以增加說服力。建議講者在演講中多分享實際案例和程式碼片段，讓聽眾更容易理解和應用這些技術。</t>
+          <t>這個提案結合了 LLM 和 RAG 技術，應用於 ESG 資訊查詢和報告生成，主題與當前趨勢相關。提案中提到了具體的 Python 套件，例如 LangChain、LlamaIndex、FlashRank、QDrantDB 和 Neo4jDB，並計劃比較不同的 LLM 模型，這顯示了一定的技術深度。然而，提案可以更深入地探討這些工具和技術在 ESG 領域的具體應用細節，例如如何處理 ESG 數據的特殊挑戰，以及如何評估不同 LLM 和 RAG 架構的性能。此外，可以考慮提供更多的實際案例或實驗數據，以增強提案的說服力。建議可以更聚焦在 Python 生態系在 ESG 領域的應用，並深入探討技術細節。</t>
         </is>
       </c>
       <c r="W50" t="inlineStr">
@@ -7686,12 +7690,12 @@
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>The proposal introduces a developer portal concept but needs more Python-specific details and concrete examples to be a strong fit for PyCon. More technical depth and practical applications are needed.</t>
+          <t>The proposal introduces a developer portal designed to improve developer experience by centralizing access to Python libraries, data APIs, and best practices. It aims to boost productivity and foster a developer community.</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>This proposal discusses the creation of a developer portal to enhance developer experience, focusing on Python libraries and data engineering. While the concept is relevant, the proposal needs more specific examples of how Python is used within the portal and how it directly benefits Python developers. The outline is a bit high-level and could benefit from more concrete examples and technical details. Consider adding more details on the Python libraries and frameworks used, and how the portal streamlines Python development workflows. Also, clarify the target audience; is it for developers building the portal or using it? More focus on the 'how' rather than the 'why' would be beneficial.</t>
+          <t>This proposal discusses the creation of a developer portal to enhance developer experience, focusing on Python libraries and data engineering. While the concept is relevant, the proposal needs to provide more specific examples of how Python is used within the portal and how it benefits Python developers. The outline is clear, but the technical depth related to Python needs to be increased. Consider adding more details on the Python libraries, frameworks, and data pipeline construction aspects. Also, clarify the innovative aspects of your approach. Without these improvements, the proposal is somewhat generic.</t>
         </is>
       </c>
       <c r="W51" t="inlineStr">
@@ -7818,12 +7822,12 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>提案結合 Python 和自駕車技術，但技術深度稍嫌不足，建議加強技術細節和實用性。</t>
+          <t>本提案介紹使用 CARLA 模擬器和 Python API，搭配 OpenCV 和 TensorFlow，以 DDPG 演算法訓練自駕車系統。內容涵蓋環境配置、模型建立和成果展示，目標受眾為對自動駕駛和 VANET 研究感興趣的中高階 Python 使用者。</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>此提案介紹了使用 CARLA 模擬器和 Python API 進行自駕車深度強化學習的應用，並提及了 OpenCV 和 TensorFlow 等工具。優點是結合了 Python 和前沿的自駕車技術，並提供了開源模擬器的使用方法。但技術深度稍嫌不足，DDPG 演算法的介紹可以更深入，並加入更多實驗數據或案例分析。另外，VANET 的部分可以更明確地與 Python 結合。建議加強技術細節和實用性，例如展示如何使用 Python 處理 CARLA 輸出的數據，以及 DDPG 模型的具體參數和訓練過程。</t>
+          <t>此提案介紹了使用 CARLA 模擬器和 Python API 進行自駕車深度強化學習的應用。優點是結合了 Python 和前沿的自動駕駛技術，並使用了流行的開源工具如 CARLA、OpenCV 和 TensorFlow。然而，提案對於 DDPG 演算法的介紹可能過於簡略，建議增加更多關於模型架構、訓練細節以及如何處理實際駕駛挑戰的描述。此外，雖然提到了 VANET，但缺乏具體整合方案的細節。如果能更深入地探討 Python 在 VANET 整合中的作用，將會更符合 PyCon TW 的主題。</t>
         </is>
       </c>
       <c r="W52" t="inlineStr">
@@ -8022,12 +8026,14 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>提案介紹使用 Python 進行主題模型分析網路銀行 App 客戶評論，具有技術深度和實用性，但可更深入比較各種方法的優缺點。</t>
+          <t>本提案將以台灣 19 間銀行的 APP 在 Google Play 上共 31,474 筆評論為例，示範如何透過 Python 進行主題模型(Topic modeling)，從文本中萃取出不同的討論話題，並為各個話題找出有意義的重要關鍵詞，讓公司能深入了解 APP 使用體驗與優缺點。</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>這個提案探討了使用 Python 進行主題模型分析網路銀行 App 客戶評論，以了解客戶體驗和優缺點。內容涵蓋了多種主題模型方法（LDA、Word2Vec、Sentence Transformer），並深入探討了實務上會遇到的問題，例如長文本處理、可解釋性以及加速方法。提案結構清晰，大綱詳細，涵蓋了從理論到實踐的各個方面。與 PyCon 主題相關性高，具有一定的技術深度和實用性。建議可以更深入探討各種方法的優缺點比較，並提供更多實際案例。</t>
+          <t xml:space="preserve">這個提案介紹了如何使用 Python 進行主題模型分析客戶對於數位銀行 App 的評論，並從中萃取有意義的資訊。內容涵蓋了多種主題模型方法，包括傳統的 LDA 和基於大型語言模型的方法，並比較了它們的優缺點。提案也深入探討了實務上會遇到的問題，例如長文本處理和模型解釋性，並提供了相應的解決方案。整體而言，這個提案與 PyCon 的主題相關，且具備一定的技術深度和實用性。
+建議可以更具體地展示不同主題模型方法在實際資料上的效果比較，並提供更多的程式碼範例，讓聽眾更容易上手。此外，可以更深入地探討如何將主題模型分析結果應用於實際的業務決策中。
+</t>
         </is>
       </c>
       <c r="W53" t="inlineStr">
@@ -8180,12 +8186,12 @@
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>提案探討 Sync/Async 在 Web Server 效能上的差異，並使用 Locust 進行負載測試。建議深入探討 FastAPI 框架在 Async 上的應用細節，並提供更多實際的程式碼範例和實驗數據。</t>
+          <t>本提案以 FastAPI 為例，使用 Locust 進行負載測試，比較 Sync 和 Async 在處理 I/O Bound 和 CPU Bound 任務時的效能差異。探討了使用 Gunicorn、Nginx 和 Celery 進行最佳化的方向。</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>這個提案探討了 Sync 和 Async 在 Web Server 效能上的差異，並使用 Locust 進行負載測試，這是一個很有趣且實用的主題。提案中提到了 I/O bound 和 CPU bound 任務，以及使用 Gunicorn、Nginx 和 Celery 進行最佳化的方向，這些都是很好的切入點。建議可以更深入地探討 FastAPI 框架在 Async 上的應用細節，並提供更多實際的程式碼範例。此外，可以更詳細地說明如何使用 Locust 進行負載測試，以及如何分析測試結果。如果能提供更多實驗數據，會更有說服力。</t>
+          <t>這個提案探討了 Sync 和 Async 在 Web Server 效能上的差異，並使用 Locust 進行負載測試，對於想了解 Async 技術的 Python 使用者來說很有幫助。建議可以更深入探討 FastAPI 框架中 Async 的具體實作細節，並提供更多實際案例或實驗數據來支持結論。此外，可以更明確地說明如何將 Load Testing 整合到開發流程中，以提升實用性。</t>
         </is>
       </c>
       <c r="W54" t="inlineStr">
@@ -8306,12 +8312,12 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>利用 Python 開源套件結合 STT 和 LLM 技術，解決電話錄音稽核痛點。建議深入探討中英文混雜校正、評測一致性方法，並分享更多資料分析細節。</t>
+          <t>本提案介紹如何利用 STT 和 LLM 技術，透過 Python 開源套件建構自動化電話錄音評測系統，將語音轉成文字後，再透過 LLM 進行評測，解決稽核流程耗時的問題，提升生產效率。</t>
         </is>
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>此提案展示了如何利用 Python 開源套件（如 Whisper、pyannote、Langchain）結合 STT 和 LLM 技術，解決電話錄音稽核的痛點，並提升生產力。優點是問題明確、解決方案完整，並提供程式碼和 Demo。建議可以更深入探討中英文混雜校正的具體方法，以及如何利用 Langchain 確保評測一致性。另外，可以分享更多關於資料分析和 Metabase 的應用細節。總體而言，此提案與 PyCon 主題相關性高，具有實用價值。</t>
+          <t>這個提案展示了如何使用 Python 和相關的開源工具（如 Whisper、pyannote、Langchain）來自動化電話錄音評測，從而顯著提高生產力。優點是結合了 STT 和 LLM 技術，並提供了實際的應用案例。建議可以更深入地探討程式碼實現細節，例如如何處理中英文混雜的校正問題，以及如何優化 LLM 評測的一致性。此外，可以分享更多關於數據分析和 Metabase 的使用經驗。總體而言，這個提案與 PyCon 主題相關，並具有一定的實用價值。</t>
         </is>
       </c>
       <c r="W55" t="inlineStr">
@@ -8466,12 +8472,12 @@
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>The proposal is relevant to PyCon, covering anti-bot systems and web scraping. Adding Python-specific examples and code snippets would enhance its appeal.</t>
+          <t>This talk explores anti-bot systems, focusing on defence layers, reputation scores, evasion strategies, and reverse engineering techniques. It aims to equip attendees with the knowledge to navigate and understand these protective measures, particularly in the context of web scraping.</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>This proposal dives into the increasingly relevant topic of anti-bot systems and web scraping, which is highly pertinent given the rise of LLMs. The outline is well-structured, covering essential aspects like defense layers, reputation scores, evasion strategies, and reverse engineering. The inclusion of practical examples, such as Javascript deobfuscation, adds significant value. However, the proposal could benefit from explicitly mentioning Python libraries or tools used in the process, such as Scrapy, Selenium, or requests-html, to strengthen its connection to the PyCon audience. Also, elaborating on how these techniques can be implemented within a Python-centric workflow would be beneficial. Consider adding more specific examples of Python code snippets or demonstrating how Python libraries can be used to interact with and bypass anti-bot systems. This would make the presentation more directly relevant and appealing to the PyCon audience.</t>
+          <t>This proposal dives into the interesting topic of anti-bot systems and web scraping, which is relevant given the increasing use of Python in these areas. The outline is well-structured, covering defence layers, reputation scores, evasion strategies, and reverse engineering. The inclusion of practical examples and open-source tools is a plus. However, the proposal could benefit from explicitly mentioning the use of Python libraries or frameworks used in the process of bypassing anti-bot systems. Adding more details on how Python is specifically used in each step would strengthen the connection to the PyCon audience. Also, while the speaker mentions experience with web scraping and anti-bot measures, it would be beneficial to include specific examples of Python code or scripts used in their work. This would make the presentation more tangible and valuable for attendees. Consider adding more Python-specific content and examples to enhance the proposal's relevance to PyCon.</t>
         </is>
       </c>
       <c r="W56" t="inlineStr">
@@ -8671,13 +8677,12 @@
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>提案以 live-coding 方式展示網頁爬蟲技術，並提及法律注意事項。建議更明確說明 Scrapoxy 用法，並與 Python 生態系統結合，提供更多實際案例。</t>
+          <t>A live-coding session on web scraping with Python, focusing on overcoming anti-bot measures using Scrapoxy and legal considerations. Includes a dedicated website for demonstration and covers techniques like code deobfuscation and proxy management.</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>這個提案很有趣，以 live-coding 方式展示如何使用 Scrapoxy 進行網頁爬蟲，並克服反爬蟲機制。對於想要學習網頁爬蟲技術的開發者來說，會很有幫助。提案中也提到了法律相關的注意事項，這點很好。不過，可以更明確地說明 Scrapoxy 的具體用法，以及如何與 Python 的其他網頁爬蟲框架（如 Scrapy）整合。另外，可以考慮提供更多實際案例，展示如何使用這些技術來解決實際問題。
-如果能更深入探討 Python 在整個流程中所扮演的角色，以及如何利用 Python 的生態系統來提升網頁爬蟲的效率和可靠性，會更符合 PyCon 的主題。</t>
+          <t>This proposal outlines a live-coding session on web scraping using Python and Scrapoxy. It covers important aspects like overcoming anti-bot measures and legal considerations. The live-coding format is engaging, and the use of a dedicated website for demonstration is a plus. However, the proposal could benefit from more specific details on the Python libraries used (beyond Scrapy) and a deeper dive into the code deobfuscation techniques. While it mentions Playwright, elaborating on its integration with Scrapoxy would enhance the technical depth. The legal section should be expanded to provide more concrete guidance. Consider adding more details on how the AI models will be trained using the scraped data to strengthen the connection to practical applications. Also, the outline seems a bit rushed, especially the live challenge-solving part. Consider allocating more time to the more complex challenges. Finally, while the narrative is engaging, ensure the focus remains on the technical aspects of web scraping with Python.</t>
         </is>
       </c>
       <c r="W57" t="inlineStr">
@@ -8827,12 +8832,12 @@
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>The proposal presents a compelling application of NetworkX for economic network analysis, specifically the World Trade Network. It's well-structured and includes a hands-on demo. Adding more details on challenges and actionable insights would strengthen the proposal.</t>
+          <t>The proposal explores economic phenomena through network science, focusing on the World Trade Network. It uses NetworkX, Pandas, and Matplotlib to analyze trade data for commodities like Natural Gas, Coffee, and Diamonds, demonstrating network density, heterogeneity, and centrality measures.</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>This proposal effectively combines economic theory with practical Python implementation using NetworkX. It clearly outlines the use of Python libraries for network analysis of the World Trade Network. The hands-on demonstration using the BACI-CEPII dataset is a strong point. However, the proposal could benefit from elaborating on the challenges encountered and solutions implemented during the network analysis. Also, it would be good to mention the specific versions of the libraries used. Consider adding more details on how the analysis provides actionable insights for economic policy or business strategy. The target audience is well-defined, but the level of prior knowledge assumed might be a bit high; consider adding a brief introduction to network science concepts for those less familiar.</t>
+          <t>This proposal introduces network analysis in economics using Python's NetworkX library. It covers the World Trade Network and analyzes specific commodities. The talk is well-structured with a clear outline and hands-on demonstration. However, the proposal could benefit from highlighting specific challenges or novel insights gained from the analysis. Also, while it mentions several Python libraries, it could elaborate on the specific Pythonic solutions or techniques used to address the challenges in network analysis. Consider adding more details on how Python facilitates the analysis and visualization of the economic data.</t>
         </is>
       </c>
       <c r="W58" t="inlineStr">
@@ -8965,12 +8970,12 @@
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>提案探討 Python 環境遷移問題，具有實用價值，但可更深入探討跨平台依賴處理和提供更多案例。</t>
+          <t>本提案介紹如何將 Python 程式碼的環境遷移到其他地方，包括 virtualenv/conda env 的原理、打包 virtualenv 的方法，以及利用現成工具打包 Python 程式和其依賴。目標是幫助開發者在離線或低網速環境配置 Python 環境，並簡化 Python 應用程式部署流程。</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>這個提案探討了 Python 環境遷移的問題，包括 virtualenv 和 conda env 的原理以及如何將環境轉移到其他系統。議程涵蓋了底層實作和應用實作，並提及了相關工具如 beeware, pyinstaller, shiv 等。對於需要在離線或低網速環境部署 Python 應用程式的開發者來說，這個議題具有一定的實用價值。然而，提案可以更深入地探討跨平台依賴處理的具體方法，並提供更多實際案例或實驗數據來支持其觀點。此外，可以更詳細地介紹各個工具的優缺點和適用場景，以便聽眾更好地選擇適合自己的方案。</t>
+          <t>這個提案探討了 Python 環境遷移的問題，對於需要在不同環境部署 Python 程式碼的開發者來說相當實用。提案涵蓋了 virtualenv 和 conda env 的原理，以及將環境打包成單一執行檔的工具，具有一定的技術深度。建議可以更深入探討跨平台依賴處理的細節，並提供更多實際案例或實驗數據來支持論點。此外，可以更明確地說明各種工具的優缺點，幫助聽眾選擇最適合自己的方案。</t>
         </is>
       </c>
       <c r="W59" t="inlineStr">
@@ -9096,17 +9101,17 @@
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>The proposal offers practical Docker optimization techniques for Python applications, making it relevant and useful. Adding performance metrics and more specific examples would strengthen the proposal.</t>
+          <t>The proposal outlines practical tactics for building fast, minimal Python Docker images using techniques like uv, multi-stage builds, and caching. It aims to help Python developers optimize their Dockerfiles for improved build times and reduced image sizes.</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>This proposal focuses on practical techniques for optimizing Python Docker images, which is highly relevant to many Python developers. The use of tools like uv and multi-stage builds is a good sign. The outline is clear and the objective is well-defined. It would be beneficial to include specific examples of the performance improvements achieved with each tactic (e.g., reduced image size, faster build times). Also, consider elaborating on the challenges encountered and how they were overcome. Mentioning specific Python frameworks or libraries used in the example application would also add value.</t>
+          <t>This proposal focuses on practical techniques for optimizing Python Docker images, which is highly relevant to many Python developers. The use of uv and other optimization strategies is well-aligned with improving workflow and productivity. The outline is clear and the objective is well-defined. It would be beneficial to include specific examples or benchmarks to demonstrate the effectiveness of each tactic. Also, consider elaborating on the challenges and trade-offs associated with each optimization technique.</t>
         </is>
       </c>
       <c r="W60" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>+1</t>
         </is>
       </c>
       <c r="X60" t="inlineStr">
@@ -9246,12 +9251,18 @@
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>分享了在醫療資訊系統中利用 Python 逐步整合微服務的實務經驗，對有類似需求的開發者有參考價值。建議深入探討技術細節和測試部署策略。</t>
+          <t>分享在醫院環境中，如何使用 Python 逐步將新微服務與既有系統無縫串接的策略與技術手段，涵蓋新舊系統資料互通、跨語言服務溝通及服務不中斷更新等議題。適合對微服務導入單體系統有興趣的資訊主管或工程師。</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>這個提案分享了在醫療資訊系統中，如何使用 Python 逐步新增微服務並與舊系統整合的實務經驗，包括與 Delphi、PHP 和 4GL 系統的介接。內容涵蓋了技術選型、資料互通、服務不中斷更新等多個方面，對於有類似需求的開發者或主管具有參考價值。建議可以更深入地探討特定技術挑戰的解決方案，例如罕見字編碼處理的細節，以及不同系統間溝通的具體程式碼範例。此外，可以考慮加入更多關於測試和部署策略的討論。</t>
+          <t>這個提案分享了在醫院環境中，如何使用 Python 逐步將新微服務與既有系統（Delphi, PHP, 4GL based）無縫串接的策略與技術手段。內容涵蓋了新舊系統資料互通、Python 服務與其他語言服務之間的溝通，以及版本更新不中斷的技術。提案中提到了 pyodbc、Flask、APIFlask、Docker 等技術，並分享了在實際應用中遇到的困難與解決方案。雖然實作細節可能不多，但對於有類似需求的資訊主管或工程師來說，具有一定的參考價值。建議可以更深入地探討特定技術的實作細節，例如罕見字編碼的處理、Delphi 內嵌 Python 微服務的具體方法等。
+優點：
+* 實際案例分享，具有一定的實用性。
+* 涵蓋多種技術棧的整合，具有一定的廣度。
+缺點：
+* 技術深度可以再加強，可以更深入地探討特定技術的實作細節。
+* 缺乏具體的效能數據或實驗結果，說服力稍嫌不足。</t>
         </is>
       </c>
       <c r="W61" t="inlineStr">
@@ -9389,12 +9400,12 @@
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>提案介紹了基於 Raspberry Pi 和 Python 的 DuckieDrone 無人機專案，涵蓋多個 Python 套件的應用。建議加入更多程式碼範例和實驗數據。</t>
+          <t>介紹使用 Raspberry Pi 和 Python 打造的 DuckieDrone 無人機專案，涵蓋硬體、飛控、感測器、ROS 和 Python 控制等技術細節。建議深入探討技術實作細節，並加入更多專案實例或實驗數據。</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>這個提案介紹了使用 Raspberry Pi 和 Python 打造 DuckieDrone 無人機專案，涵蓋了 ROS、Numpy、OpenCV 和 GPIO 等多個 Python 套件的應用。內容涉及硬體控制、感測器數據處理、姿態估計和 PID 控制等技術細節，與 PyCon 主題相關性高。如果能更深入地探討這些 Python 套件在無人機控制中的具體應用和遇到的挑戰，會更有吸引力。建議在演講中加入更多實際的程式碼範例和實驗數據，以增強說服力。</t>
+          <t>這個提案介紹了使用 Raspberry Pi 和 Python 打造小型無人機專案 DuckieDrone，將機器人技術從二維延伸到三維空間。內容涵蓋了硬體選擇、飛控原理、感測器應用、ROS 和 Python 控制，以及濾波演算法和 PID 控制等技術細節。提案明確列出了使用的 Python 套件，如 ROS、Numpy、OpenCV 和 GPIO。優點是結合了軟硬體，並提供了實際的 Python 應用範例。建議可以更深入探討特定技術的實作細節，例如 PID 控制器的參數調整、Kalman 濾波的具體應用，以及在無人機上的實際效果。此外，可以考慮加入更多專案實例或實驗數據，以增強說服力。</t>
         </is>
       </c>
       <c r="W62" t="inlineStr">
@@ -9525,12 +9536,12 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>The proposal introduces GeoDjango for geo-enabled web applications. It's relevant but could benefit from more technical depth, implementation details, and a more detailed outline.</t>
+          <t>This proposal introduces GeoDjango for developing geo-enabled web applications. It covers storing geographic data, performing geographic queries, and building a location-based application with Django. The talk aims to demonstrate the ease of use and versatility of GeoDjango.</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t xml:space="preserve">This proposal introduces GeoDjango, a framework for developing web applications with geographic data capabilities. It highlights the ease of use and versatility of GeoDjango for handling geographic data and performing geographic queries. The talk aims to demonstrate how to develop a location-enabled application with an example, showcasing features like adding pins with messages and photos on a map, and performing complex searches. While the proposal focuses on a specific Django extension, it could benefit from elaborating on the challenges and solutions encountered during the implementation of the example application. Adding more details on specific Python libraries used and their integration with GeoDjango would also enhance the technical depth. Consider including performance considerations or optimization techniques for handling large geographic datasets. Also, the outline seems a bit short, consider adding more details to each section. </t>
+          <t>This proposal introduces GeoDjango, a framework for developing web applications with geographic data capabilities. It highlights the ease of use and versatile functionality of GeoDjango for handling geographic data and performing geographic queries. The talk aims to demonstrate how to develop a location-enabled application with an example, including adding pins with messages and photos on a map and performing complex searches. The outline is clear and covers the necessary aspects of GeoDjango. However, the proposal could benefit from more specific details on the challenges and solutions encountered during the implementation of the example application. Also, elaborating on the Python-specific aspects and the depth of Django usage would strengthen the proposal's relevance to PyCon. Consider adding more details on the specific geographic queries and data handling techniques used within Django.</t>
         </is>
       </c>
       <c r="W63" t="inlineStr">
@@ -9657,12 +9668,12 @@
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>The proposal is relevant and practical, demonstrating how to build custom linters using the `ast` module. Clarifying the purpose and benefits of 'un-pythonic' code enforcement would improve the proposal.</t>
+          <t>The proposal introduces how to use the `ast` module to build a custom linter for enforcing specific code styles, potentially 'un-pythonic' ones, using real-world examples and pre-commit integration. It aims to help developers understand code analysis and customize linting tools.</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>This proposal presents a practical application of the `ast` module for building custom linters, which is highly relevant to Python developers. The real-world example from Apache Airflow adds credibility. However, the title and some descriptions lean towards 'un-pythonic' code, which might confuse the audience. Clarifying the purpose (e.g., enforcing specific project conventions or dealing with legacy code) would be beneficial. The outline is clear and well-structured. Consider emphasizing the benefits of custom linters in specific scenarios.</t>
+          <t>This proposal focuses on using the `ast` module to build a custom linter, which is highly relevant to Python developers. It provides practical knowledge on code analysis and customization of linting tools. The real-world example and the integration with pre-commit enhance the proposal's value. However, the title and some descriptions lean towards being 'un-pythonic,' which might confuse some audience members. Clarifying the purpose and benefits of creating such a linter (e.g., for specific legacy code constraints or educational purposes) would improve the proposal. Consider emphasizing the practical applications and benefits more clearly.</t>
         </is>
       </c>
       <c r="W64" t="inlineStr">
@@ -9783,12 +9794,12 @@
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>Good overview of core Python features with real-world examples. Could benefit from deeper dives into implementation challenges and trade-offs.</t>
+          <t>This presentation introduces dunder methods, decorators, and iterable protocols in Python, showcasing their application in open-source projects like Apache Airflow. It aims to demonstrate the practical usage of these fundamental concepts.</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>This proposal introduces several core Python features with real-world examples from open-source projects, which aligns well with PyCon's focus on practical Python knowledge. The outline is clear and provides specific examples. However, the proposal mentions it's a brief introduction and doesn't extensively cover the details. To improve, the speaker could delve deeper into the challenges faced and solutions implemented when using these features in the mentioned projects. Also, elaborating on the benefits and trade-offs of using these features would enhance the talk's value. Consider adding more context on why these specific features were chosen over alternatives in those scenarios.</t>
+          <t>This proposal introduces several core Python features with real-world examples from open-source projects. It's a good starting point, but the presentation could benefit from a deeper dive into the challenges and solutions encountered when applying these features. Consider elaborating on the specific problems these features solved in the linked Airflow pull requests. Also, while mentioning "Learning Python, 5th Edition" is fine, try to add more original insights or perspectives. To improve, focus on providing more in-depth explanations and practical takeaways for the audience. Consider adding more code snippets to illustrate the concepts.</t>
         </is>
       </c>
       <c r="W65" t="inlineStr">
@@ -9939,12 +9950,12 @@
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>提案介紹了使用 RAG 技術建立勞動法律知識問答系統，涵蓋技術選型、系統架構和實作細節。建議更深入探討法律領域的特殊挑戰，並加入更多實際案例。</t>
+          <t>本提案介紹使用 RAG 技術建立勞動法律知識問答系統，採用 OpenAI 模型，並針對法律領域的特殊性進行優化。展示了系統架構、實作細節和 Streamlit 介面。</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>這個提案介紹了使用 RAG 技術建立勞動法律知識問答系統，選用 OpenAI embedding 和 GPT-4，並探討了文本前處理、資訊檢索和生成方面的優化技巧。內容涵蓋了技術選型、系統架構和實作細節，並展示了 Streamlit 介面。對於想了解 RAG 應用和法律文本處理的聽眾來說，會是不錯的分享。建議可以更深入探討法律領域的特殊挑戰，例如如何處理法律條文的模糊性和多義性。可以考慮加入更多實際案例，展示系統在解決複雜法律問題上的能力。</t>
+          <t>這個提案介紹了如何使用 RAG 技術來建立一個勞動法律知識問答系統，選用了 OpenAI 的詞嵌入模型和 GPT-4，並探討了在法律領域應用 RAG 時遇到的挑戰和優化策略，例如結合標籤系統、Prompt Engineering 等。內容涵蓋了技術選型、系統架構和實作細節，並展示了 Streamlit 介面。整體而言，與 PyCon 主題相關性高，且具有一定的技術深度和實用性。建議可以更深入探討 Python 在整個系統中的角色，例如資料處理、模型部署等方面。可以考慮將更多的開源工具和框架納入討論，並比較它們的優缺點。</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
@@ -10077,12 +10088,12 @@
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>提案結合 LLM 與不實資訊偵測，具備潛力。建議加強實作細節、提供更多案例，並聚焦 Python 程式碼。</t>
+          <t>本提案介紹如何使用 Python 和 LangChain 建立 LLM Agent，自動偵測台灣 2024 總統大選的不實資訊。將分享不實資訊技術的趨勢，以及透過 LangChain 使用 LLM 的方法，並理解這些技術如何識別和對抗資訊操弄。</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>這個提案結合了 LLM 和不實資訊偵測，是一個有趣且與時事相關的議題。使用 LangChain 框架串接流程，並以 Python 實作，符合 PyCon 的主題。然而，提案可以更深入地探討 Agent 模組的實作細節，例如如何利用 DISARM 框架進行不實資訊偵測，以及如何優化偵測策略。此外，可以提供更多實際案例或實驗數據，以增強內容的說服力。如果能更聚焦在 Python 程式碼的展示與解釋，會更符合 PyCon 受眾的需求。</t>
+          <t>這個提案結合了 LLM 和不實資訊偵測，是一個有趣且與時事相關的議題。使用 LangChain 框架串接流程，並以 Python 實作，符合 PyCon 的主題。建議可以更深入探討 Agent 在偵測過程中的具體演算法和判斷依據，以及如何評估偵測結果的準確性。另外，可以考慮分享更多實際案例，例如偵測到的具體不實資訊類型和應對策略。如果時間允許，可以加入更多程式碼範例，讓聽眾更容易上手。</t>
         </is>
       </c>
       <c r="W67" t="inlineStr">
@@ -10232,12 +10243,13 @@
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>The proposal covers data validation and ETL testing with relevant frameworks. More Python-specific examples would strengthen its fit for PyCon.</t>
+          <t>The proposal discusses data validation and ETL pipeline testing, emphasizing the importance of data integrity in AI. It introduces frameworks like Great Expectations and dbt for automating data testing, aiming to equip data engineers and scientists with the knowledge to implement robust data validation strategies.</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>This proposal introduces data validation and ETL pipeline testing, which are crucial for AI applications using Python. It covers frameworks like Great Expectations and dbt, offering practical tools for data engineers and scientists. However, the proposal could benefit from more specific examples of how these frameworks are used within Python code and how they address particular data challenges. Detailing the integration of these tools within a Python-centric workflow would enhance its relevance to the PyCon audience.</t>
+          <t xml:space="preserve">This proposal provides a good overview of data validation and ETL testing, which are crucial for AI applications using Python. The inclusion of frameworks like Great Expectations and dbt is relevant. However, the proposal could benefit from more specific examples of how these frameworks are used in Python code, and perhaps a deeper dive into the challenges and solutions encountered when implementing these techniques in real-world Python-based data pipelines. Consider adding more concrete Python code snippets or case studies to enhance the practical value for the audience. Also, while the target audience is well-defined, consider tailoring the examples to specific Python-centric data science or engineering tasks.
+</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
@@ -10354,12 +10366,12 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>The proposal introduces Perspective for high-performance data visualization. It's well-structured and practical, but could benefit from a deeper focus on Python-specific aspects.</t>
+          <t>This talk introduces Perspective, a high-performance data visualization component, and demonstrates its integration with FastAPI for building web frontends with features like pivoting, sorting, filtering, and real-time data updates.</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>This proposal introduces Perspective, a high-performance data visualization component, and demonstrates its integration with FastAPI for building web frontends. The talk covers essential features like pivoting, sorting, filtering, and real-time data updates. The outline is well-structured, and the objective is clear: to empower users to create flexible UIs using open-source tools. While the proposal highlights the use of Python, C++, Rust, JavaScript, and WebAssembly, it could benefit from a deeper dive into the Python-specific aspects and challenges encountered during integration. More emphasis on the Python API and its usage would strengthen the proposal's relevance to the PyCon audience.</t>
+          <t>This proposal introduces Perspective, a high-performance data visualization component, and demonstrates its integration with FastAPI for building web frontends. The talk covers essential features like pivoting, sorting, filtering, and real-time data updates. The speaker also plans to show how to use Perspective and incorporate it into applications for both static and streaming data. The proposal clearly outlines the talk's structure and objectives, making it easy to follow. The use of Python, along with C++, Rust, and WebAssembly, aligns well with the PyCon audience's interests. However, the proposal could benefit from more specific examples of how Perspective addresses common data visualization challenges in Python-based web applications. Also, elaborating on the performance benefits compared to other Python visualization libraries would strengthen the proposal. Consider adding more details on the specific Python APIs used and how they interact with the underlying C++/Rust code. Also, consider adding more details on how Perspective handles large datasets and streaming data in a Python environment. This would make the proposal more appealing to the PyCon audience.</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
@@ -10482,19 +10494,17 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>提案介紹使用 Jupyter Notebooks 產生高品質印刷文章的方法，展示了 Python 在生成印刷媒體方面的應用。具有實用性和創新性，適合 PyCon 的受眾。</t>
+          <t>本提案介紹使用 Jupyter Notebook 和 nbprint 生成印刷品質文章的方法，重點介紹了 nbprint 和 paged.js 這兩個工具，並展示了如何將 Notebook 轉換為新聞文章、教科書和商業報告等印刷媒體。</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t xml:space="preserve">這個提案介紹了使用 Jupyter Notebooks 產生高品質印刷文章的方法，聚焦於相關的 libraries 和工具，例如 nbprint 和 paged.js。這與 PyCon 的主題相關，展示了 Python 在生成印刷媒體方面的應用。提案中包含實際案例和技術細節，例如配置和運行參數化報告。講者也提到了未來的工作和潛在應用，例如使用 LLMs 產生客製化文件。這個提案具有實用性和創新性，適合 PyCon 的受眾。
-建議講者在 demo 環節中，更詳細地展示 nbprint 的配置和使用方法，以及如何解決在生成印刷媒體時可能遇到的問題。此外，可以更深入地探討如何將 LLMs 應用於生成客製化文件，例如自動生成新聞報導或商業報告。
-</t>
+          <t>這個提案很有趣，展示了 Jupyter Notebook 在生成印刷品質文件方面的潛力，特別是通過 nbprint 和 paged.js 的結合。這對於需要生成報告、教科書或新聞文章的用戶來說非常實用。建議可以更深入地探討 nbprint 的具體配置和使用案例，以及如何解決在實際應用中可能遇到的問題。此外，可以考慮展示更多不同類型的印刷媒體案例，以擴大受眾的視野。</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="X70" t="inlineStr">
@@ -10644,12 +10654,12 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>Good introduction to Pygame for beginners with live coding. Suggest adding more Pythonic details and tailoring content for PyCon TW.</t>
+          <t>This talk introduces game programming with Pygame, covering fundamentals like collision detection and game loops through live coding. It aims to inspire students, but lacks technical depth and specific examples.</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>This proposal introduces game programming with Pygame, which can be engaging for beginners. The live coding aspect and audience participation are strong points. However, the proposal could benefit from more details on specific Pythonic solutions or advanced Pygame techniques. Consider elaborating on how Pygame integrates with other Python libraries or frameworks. Also, while the talk has been given before, highlighting any new content or adaptations for the PyCon TW audience would be beneficial.</t>
+          <t>The proposal introduces Pygame, a game programming library for Python, and aims to demonstrate game programming fundamentals through live coding. While the topic can be engaging, the proposal lacks depth regarding specific challenges and solutions encountered during game development. The outline is basic and could benefit from more details on the game programming patterns and collision detection techniques used. To improve, the talk could include more advanced Pygame features or explore optimization strategies. The live coding aspect is a plus, but the proposal should clarify how audience participation will be integrated effectively. Consider adding more specific examples of how Python is central to the game development process. The speaker mentions having given this talk before, which is a plus, but it would be good to know how the talk has evolved based on previous feedback.</t>
         </is>
       </c>
       <c r="W71" t="inlineStr">
@@ -10788,12 +10798,12 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>提案將 RAG 技術應用於資安事件分析，具備實用性。但 Python 技術深度可再加強，建議提供更多程式碼範例和實作案例。</t>
+          <t>本提案旨在將 RAG 技術應用於資安事件分析，利用 LLaMA2 和 QLoRA 微調模型，並結合 Gradio, LLaMA-Factory, LangChain 等工具，協助資安分析師快速獲取有價值的資訊。目標受眾包括資安分析師、非 ML 專業人士和學生。</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>這個提案結合了 RAG 技術與資安事件分析，具有一定的實用性。使用了 LLaMA2 和 QLoRA 微調模型，並考量了資料隱私，這點值得肯定。然而，提案中關於 Python 的技術深度可以再加強，例如更深入地探討 LangChain 在 RAG 中的應用，以及如何使用 Pytorch 進行模型微調。此外，可以提供更多實際的程式碼範例，讓聽眾更容易上手。建議可以更聚焦在 Python 相關的技術細節，並提供更多實作案例。</t>
+          <t>這個提案結合了 RAG 技術與資安事件分析，選題具有一定的實用性。使用了 LLaMA2 和 QLoRA 微調模型，並考慮到商業應用和資料隱私，這是一個優點。提案中提到了 Gradio, LLaMA-Factory, LangChain 等工具，並給出了連結，方便參考。大綱也算清晰，涵蓋了 RAG 介紹、資安背景和總結。然而，技術深度可以再加強，例如更詳細地介紹模型微調的過程、RAG 的具體實作細節，以及如何解決實際資安分析中遇到的挑戰。另外，可以考慮加入更多實際案例或實驗數據，以增強說服力。可以更明確地說明如何使用 Python 程式碼介接 LLM，並展示具體的程式碼範例。總體而言，這個提案具有潛力，但需要進一步完善技術細節和實用性。</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
@@ -10929,12 +10939,12 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>The proposal effectively demonstrates the importance of data visualization over reliance on summary statistics using the Data Morph package. Adding more Python-specific technical details would strengthen the proposal.</t>
+          <t>The talk introduces Data Morph, a Python package that visually demonstrates the limitations of relying solely on summary statistics by morphing datasets while preserving statistical properties. It discusses the package's implementation, limitations, and lessons learned from its development.</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>This proposal effectively highlights the dangers of relying solely on summary statistics, a crucial point for data analysis. The introduction of the Data Morph package is a practical way to demonstrate this. The talk structure is well-defined, progressing from basic statistical concepts to the package's implementation and limitations. The inclusion of lessons learned from open-source development adds another layer of value. However, the proposal could benefit from emphasizing the specific Python libraries used within Data Morph (e.g., NumPy, SciPy) and showcasing how they are applied to achieve the morphing effect. This would increase the Python-specific technical depth. Consider adding a brief demo or interactive element to further engage the audience.</t>
+          <t>This proposal introduces Data Morph, a Python package that visually demonstrates the limitations of relying solely on summary statistics. It's a good topic for illustrating statistical concepts in an engaging way. The talk includes a practical demonstration of the package and discusses its implementation. However, the proposal could benefit from emphasizing the specific Python libraries used (e.g., visualization libraries) and how they are integrated within the Data Morph package. Also, while the talk mentions open-source contributions, it could be strengthened by detailing the specific challenges and solutions encountered during the development of the package, particularly those related to Python. Consider adding more details on how the package leverages Python's capabilities for data manipulation and visualization. The 'Lessons Learned' section is a good addition, but could be more focused on Python-specific aspects of the project.</t>
         </is>
       </c>
       <c r="W73" t="inlineStr">
@@ -11057,12 +11067,12 @@
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>A practical guide to open source contributions with Python, offering valuable insights for beginners. Could be strengthened with more specific examples and guidance.</t>
+          <t>An introductory talk on how to get started with open source contributions, focusing on Python projects. It covers finding projects, tailoring contributions, and making the contribution itself, drawing from the speaker's experience.</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>This proposal is a good introduction to open source contributions, particularly within the Python ecosystem. It provides practical advice and examples from the speaker's experience. The outline is well-structured and covers key aspects of getting started. To improve, the talk could benefit from more specific examples of the challenges faced and how they were overcome, as well as more concrete guidance on navigating the contribution process (e.g., using Git, interacting with maintainers).</t>
+          <t>This proposal is a good introduction to open source contributions, particularly for those new to the process. It provides practical advice and examples from the speaker's experience with popular Python libraries. However, it could benefit from more specific details on the technical aspects of contributing, such as using Git, understanding code review processes, and navigating project-specific contribution guidelines. Adding a brief demo or live example could also enhance the talk's appeal. Consider focusing more on the Python-specific aspects of contributing to Python projects to strengthen its relevance to PyCon. Also, the outline seems a bit generic; consider adding more details about the specific challenges and solutions encountered while contributing to the mentioned libraries.</t>
         </is>
       </c>
       <c r="W74" t="inlineStr">
@@ -11194,12 +11204,12 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>Good overview of API contracts and specifications, particularly OpenAPI. Needs more Python-specific examples and a clearer focus on practical implementation for the audience to strongly align with PyCon's focus.</t>
+          <t>This talk introduces API design principles using OpenAPI, GraphQL, and AsyncAPI, emphasizing API contracts for maintainable and scalable APIs. It covers architectural constraints, contract-first vs. code-first approaches, and HTTP best practices. The target audience includes software developers and API designers aiming to improve their API development practices.</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>This proposal introduces API contracts using OpenAPI, GraphQL, and AsyncAPI. It covers important aspects like architectural constraints, contract-first vs. code-first approaches, and HTTP concepts. The hands-on section focusing on OpenAPI is a plus. However, the proposal could benefit from more specific Python examples, especially regarding FastAPI integration for documentation and unit testing. Also, while GraphQL and AsyncAPI are mentioned, the depth of coverage seems less than OpenAPI. Consider expanding on these or focusing more tightly on OpenAPI and its Python implementations. The outline is a bit vague in terms of concrete deliverables for the audience.</t>
+          <t>This proposal provides a good overview of API design principles and the use of OpenAPI, GraphQL, and AsyncAPI. It highlights the importance of API contracts and best practices for building maintainable and scalable APIs. The outline is well-structured, and the objective is clearly defined, targeting a broad audience of software developers and API designers. However, the proposal could benefit from more concrete Python-specific examples, particularly demonstrating how to implement these concepts using popular Python frameworks like FastAPI or Django REST framework. The hands-on section should include practical code snippets and real-world use cases to enhance the learning experience. To improve the proposal, consider adding more details on how to integrate OpenAPI specifications into Python projects and how to automate API documentation generation using tools like Swagger UI or ReDoc. Also, elaborate on the challenges and solutions encountered when adopting a contract-first approach in Python API development.</t>
         </is>
       </c>
       <c r="W75" t="inlineStr">
@@ -11332,12 +11342,12 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>Addresses model drift in ML, covering detection and management with Python tools. Could benefit from more specific examples and deeper dives into Python implementations of statistical tests and retraining strategies.</t>
+          <t>The proposal discusses model drift, its impact on machine learning models, and methods for detection and management using Python tools like scikit-multiflow and Evidently AI. It aims to provide practical knowledge for data scientists and ML engineers to maintain optimal model performance.</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>This proposal addresses a critical issue in machine learning: model drift. It clearly outlines the problem, different types of drift, and methods for detection and management, including the use of Python tools like scikit-multiflow and Evidently AI. The inclusion of a demonstration is a strong point. However, the proposal could benefit from more specific examples of how these tools are used in practice and the challenges encountered. Also, while the outline mentions statistical tests, elaborating on the Python implementation of these tests would enhance the technical depth. Consider adding more details on retraining strategies and their Pythonic implementation. The target audience is well-defined. Overall, a valuable topic for PyCon attendees.</t>
+          <t>This proposal addresses a critical issue in machine learning: model drift. It clearly outlines the problem, different types of drift, and methods for detection and management. The inclusion of Python tools like scikit-multiflow and Evidently AI is a strong point, providing practical value for attendees. The demo using Evidently AI will be particularly helpful. The talk is well-structured with a clear outline and objectives. To improve, the proposal could benefit from more specific examples of how model drift has impacted real-world applications and the solutions implemented. Also, consider adding more details on the challenges of implementing these drift detection methods in production environments. The target audience is well-defined, and the talk's content aligns well with the PyCon audience interested in practical machine learning applications.</t>
         </is>
       </c>
       <c r="W76" t="inlineStr">
@@ -11470,12 +11480,12 @@
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>The proposal presents a practical approach to web game development using Pygame and WebAssembly. Adding more technical depth and real-world examples would strengthen the proposal.</t>
+          <t>This talk explores using Pygame and PyBag to develop web-based games with WebAssembly, covering Pygame basics, WebAssembly's role, and PyBag's bridging capabilities. It aims to enable developers to create accessible and performant web games.</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>This proposal introduces using Pygame and PyBag to create web-based games with WebAssembly. It covers the basics of Pygame, the role of WebAssembly, and how PyBag bridges Python and WebAssembly. The outline is clear, and the objective is well-defined. A live coding example would greatly enhance the talk. Consider adding more details on specific challenges and solutions encountered when converting Pygame code to WebAssembly. Also, elaborate on performance optimization techniques for web-based games. Mentioning specific Python versions and Pygame/PyBag versions would be helpful.</t>
+          <t>This proposal introduces using Pygame and PyBag to create web-based games with WebAssembly. It covers the basics of Pygame, the role of WebAssembly, and how PyBag bridges Python and WebAssembly. The outline is clear, and the objective is well-defined. A live coding example would greatly enhance the talk. The proposal could benefit from more details on specific challenges and solutions encountered when converting Pygame code to WebAssembly. Also, elaborating on performance optimization techniques for web-based games would be valuable.</t>
         </is>
       </c>
       <c r="W77" t="inlineStr">
@@ -11612,12 +11622,12 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>Interesting topic but lacks Python-specific details and practical examples. Needs stronger connection to the PyCon audience.</t>
+          <t>This proposal discusses a hybrid Black Hole and Genetic Algorithm for feature selection in multilabel classification. It aims to address the challenges of high dimensionality in machine learning tasks. The talk covers the algorithm's process, genetic algorithm operators, and case studies.</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>The proposal introduces a hybrid Black Hole and Genetic Algorithm for feature selection in multi-label classification. While the topic is interesting, the proposal lacks specific details on the Python implementation and libraries used. The outline is clear, but the connection to the PyCon audience needs to be strengthened by highlighting the Python aspects of the algorithm and its application. Consider adding examples using Python libraries like scikit-learn or similar. Also, the 'Case Studies and Results' section should showcase practical Python code and performance metrics.</t>
+          <t>The proposal introduces a hybrid Black Hole and Genetic Algorithm for feature selection in multilabel classification. While the topic is interesting, the proposal lacks specific details on the Python implementation and libraries used. To improve, the speaker should include code examples or discuss how Python libraries like scikit-learn or similar tools are used in the algorithm. The case studies should also be more specific, detailing the datasets and evaluation metrics used. Without these details, the proposal is more theoretical than practical for a PyCon audience.</t>
         </is>
       </c>
       <c r="W78" t="inlineStr">

</xml_diff>